<commit_message>
update tt (cache not generated)
</commit_message>
<xml_diff>
--- a/raw/time_tables/B.Tech 62 (btech-62)/1/1.xlsx
+++ b/raw/time_tables/B.Tech 62 (btech-62)/1/1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaurav.aggarwal\Desktop\20 Aug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fileserver2\time table\Time table Odd 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5916B6E-C2A2-4674-971E-2EF889CB51AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0439D17F-A024-4AF4-95C5-4A1F6772051C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2009,7 +2009,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2103,6 +2103,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2409,7 +2415,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2590,105 +2596,60 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2700,26 +2661,74 @@
     <xf numFmtId="0" fontId="14" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2943,10 +2952,10 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D93" sqref="D93"/>
+      <selection pane="bottomRight" activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2966,16 +2975,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="93"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="80"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -3039,7 +3048,7 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="122" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -3051,7 +3060,7 @@
       <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="97" t="s">
+      <c r="E3" s="85" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -3085,7 +3094,7 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="77"/>
+      <c r="A4" s="82"/>
       <c r="B4" s="40" t="s">
         <v>442</v>
       </c>
@@ -3095,7 +3104,7 @@
       <c r="D4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="98"/>
+      <c r="E4" s="86"/>
       <c r="F4" s="8" t="s">
         <v>18</v>
       </c>
@@ -3127,7 +3136,7 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="77"/>
+      <c r="A5" s="82"/>
       <c r="B5" s="63"/>
       <c r="C5" s="63" t="s">
         <v>523</v>
@@ -3135,7 +3144,7 @@
       <c r="D5" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="98"/>
+      <c r="E5" s="86"/>
       <c r="F5" s="40" t="s">
         <v>23</v>
       </c>
@@ -3165,7 +3174,7 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="77"/>
+      <c r="A6" s="82"/>
       <c r="B6" s="41"/>
       <c r="C6" s="63" t="s">
         <v>26</v>
@@ -3173,7 +3182,7 @@
       <c r="D6" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="98"/>
+      <c r="E6" s="86"/>
       <c r="F6" s="40" t="s">
         <v>28</v>
       </c>
@@ -3203,7 +3212,7 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="77"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="41"/>
       <c r="C7" s="63" t="s">
         <v>31</v>
@@ -3211,7 +3220,7 @@
       <c r="D7" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="98"/>
+      <c r="E7" s="86"/>
       <c r="F7" s="63" t="s">
         <v>33</v>
       </c>
@@ -3243,7 +3252,7 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="77"/>
+      <c r="A8" s="82"/>
       <c r="B8" s="40"/>
       <c r="C8" s="63" t="s">
         <v>524</v>
@@ -3251,7 +3260,7 @@
       <c r="D8" s="40" t="s">
         <v>609</v>
       </c>
-      <c r="E8" s="98"/>
+      <c r="E8" s="86"/>
       <c r="F8" s="43" t="s">
         <v>473</v>
       </c>
@@ -3281,7 +3290,7 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="77"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="40"/>
       <c r="C9" s="63" t="s">
         <v>38</v>
@@ -3289,7 +3298,7 @@
       <c r="D9" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="98"/>
+      <c r="E9" s="86"/>
       <c r="F9" s="73" t="s">
         <v>599</v>
       </c>
@@ -3319,7 +3328,7 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="77"/>
+      <c r="A10" s="82"/>
       <c r="B10" s="40"/>
       <c r="C10" s="63" t="s">
         <v>525</v>
@@ -3327,7 +3336,7 @@
       <c r="D10" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="98"/>
+      <c r="E10" s="86"/>
       <c r="F10" s="38"/>
       <c r="G10" s="40" t="s">
         <v>43</v>
@@ -3355,7 +3364,7 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="77"/>
+      <c r="A11" s="82"/>
       <c r="B11" s="40"/>
       <c r="C11" s="63" t="s">
         <v>45</v>
@@ -3363,7 +3372,7 @@
       <c r="D11" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="98"/>
+      <c r="E11" s="86"/>
       <c r="F11" s="38"/>
       <c r="G11" s="44" t="s">
         <v>474</v>
@@ -3391,7 +3400,7 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="77"/>
+      <c r="A12" s="82"/>
       <c r="B12" s="40"/>
       <c r="C12" s="40" t="s">
         <v>47</v>
@@ -3399,7 +3408,7 @@
       <c r="D12" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="98"/>
+      <c r="E12" s="86"/>
       <c r="F12" s="40" t="s">
         <v>49</v>
       </c>
@@ -3429,7 +3438,7 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="77"/>
+      <c r="A13" s="82"/>
       <c r="B13" s="41"/>
       <c r="C13" s="40" t="s">
         <v>51</v>
@@ -3437,7 +3446,7 @@
       <c r="D13" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="98"/>
+      <c r="E13" s="86"/>
       <c r="F13" s="40"/>
       <c r="G13" s="64" t="s">
         <v>53</v>
@@ -3465,7 +3474,7 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="77"/>
+      <c r="A14" s="82"/>
       <c r="B14" s="41"/>
       <c r="C14" s="40" t="s">
         <v>55</v>
@@ -3473,7 +3482,7 @@
       <c r="D14" s="63" t="s">
         <v>526</v>
       </c>
-      <c r="E14" s="98"/>
+      <c r="E14" s="86"/>
       <c r="F14" s="40" t="s">
         <v>56</v>
       </c>
@@ -3503,13 +3512,13 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="77"/>
+      <c r="A15" s="82"/>
       <c r="B15" s="41"/>
-      <c r="C15" s="100" t="s">
+      <c r="C15" s="118" t="s">
         <v>527</v>
       </c>
-      <c r="D15" s="85"/>
-      <c r="E15" s="98"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="86"/>
       <c r="F15" s="40" t="s">
         <v>58</v>
       </c>
@@ -3537,21 +3546,21 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="77"/>
+      <c r="A16" s="82"/>
       <c r="B16" s="38"/>
-      <c r="C16" s="82" t="s">
+      <c r="C16" s="91" t="s">
         <v>528</v>
       </c>
-      <c r="D16" s="106"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="100" t="s">
+      <c r="D16" s="119"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="118" t="s">
         <v>529</v>
       </c>
-      <c r="G16" s="85"/>
-      <c r="H16" s="100" t="s">
+      <c r="G16" s="77"/>
+      <c r="H16" s="118" t="s">
         <v>532</v>
       </c>
-      <c r="I16" s="85"/>
+      <c r="I16" s="77"/>
       <c r="J16" s="2"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -3571,21 +3580,21 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="77"/>
+      <c r="A17" s="82"/>
       <c r="B17" s="38"/>
-      <c r="C17" s="100" t="s">
+      <c r="C17" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="85"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="100" t="s">
+      <c r="D17" s="77"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="118" t="s">
         <v>530</v>
       </c>
-      <c r="G17" s="85"/>
-      <c r="H17" s="100" t="s">
+      <c r="G17" s="77"/>
+      <c r="H17" s="118" t="s">
         <v>533</v>
       </c>
-      <c r="I17" s="85"/>
+      <c r="I17" s="77"/>
       <c r="J17" s="2"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -3605,21 +3614,21 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="77"/>
+      <c r="A18" s="82"/>
       <c r="B18" s="38"/>
-      <c r="C18" s="88" t="s">
+      <c r="C18" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="85"/>
-      <c r="E18" s="98"/>
-      <c r="F18" s="88" t="s">
+      <c r="D18" s="77"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="89" t="s">
         <v>491</v>
       </c>
-      <c r="G18" s="85"/>
-      <c r="H18" s="88" t="s">
+      <c r="G18" s="77"/>
+      <c r="H18" s="89" t="s">
         <v>484</v>
       </c>
-      <c r="I18" s="85"/>
+      <c r="I18" s="77"/>
       <c r="J18" s="2"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -3639,21 +3648,21 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="77"/>
+      <c r="A19" s="82"/>
       <c r="B19" s="38"/>
-      <c r="C19" s="88" t="s">
+      <c r="C19" s="89" t="s">
         <v>595</v>
       </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="88" t="s">
+      <c r="D19" s="77"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="85"/>
-      <c r="H19" s="88" t="s">
+      <c r="G19" s="77"/>
+      <c r="H19" s="89" t="s">
         <v>494</v>
       </c>
-      <c r="I19" s="85"/>
+      <c r="I19" s="77"/>
       <c r="J19" s="2"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -3673,21 +3682,21 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="77"/>
+      <c r="A20" s="82"/>
       <c r="B20" s="38"/>
-      <c r="C20" s="103" t="s">
+      <c r="C20" s="97" t="s">
         <v>514</v>
       </c>
-      <c r="D20" s="85"/>
-      <c r="E20" s="98"/>
-      <c r="F20" s="103" t="s">
+      <c r="D20" s="77"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="97" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="85"/>
-      <c r="H20" s="103" t="s">
+      <c r="G20" s="77"/>
+      <c r="H20" s="97" t="s">
         <v>430</v>
       </c>
-      <c r="I20" s="85"/>
+      <c r="I20" s="77"/>
       <c r="J20" s="2"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -3707,21 +3716,21 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="77"/>
+      <c r="A21" s="82"/>
       <c r="B21" s="38"/>
-      <c r="C21" s="103" t="s">
+      <c r="C21" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="85"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="103" t="s">
+      <c r="D21" s="77"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="97" t="s">
         <v>513</v>
       </c>
-      <c r="G21" s="85"/>
-      <c r="H21" s="103" t="s">
+      <c r="G21" s="77"/>
+      <c r="H21" s="97" t="s">
         <v>428</v>
       </c>
-      <c r="I21" s="85"/>
+      <c r="I21" s="77"/>
       <c r="J21" s="2"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -3741,21 +3750,21 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="77"/>
+      <c r="A22" s="82"/>
       <c r="B22" s="40"/>
-      <c r="C22" s="107" t="s">
+      <c r="C22" s="116" t="s">
         <v>606</v>
       </c>
-      <c r="D22" s="108"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="88" t="s">
+      <c r="D22" s="117"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="G22" s="85"/>
-      <c r="H22" s="88" t="s">
+      <c r="G22" s="77"/>
+      <c r="H22" s="89" t="s">
         <v>452</v>
       </c>
-      <c r="I22" s="85"/>
+      <c r="I22" s="77"/>
       <c r="J22" s="2"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -3775,21 +3784,21 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="77"/>
+      <c r="A23" s="82"/>
       <c r="B23" s="40"/>
-      <c r="C23" s="88" t="s">
+      <c r="C23" s="89" t="s">
         <v>450</v>
       </c>
-      <c r="D23" s="85"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="88" t="s">
+      <c r="D23" s="77"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="89" t="s">
         <v>451</v>
       </c>
-      <c r="G23" s="85"/>
-      <c r="H23" s="88" t="s">
+      <c r="G23" s="77"/>
+      <c r="H23" s="89" t="s">
         <v>453</v>
       </c>
-      <c r="I23" s="85"/>
+      <c r="I23" s="77"/>
       <c r="J23" s="2"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -3809,18 +3818,18 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="77"/>
-      <c r="B24" s="88" t="s">
+      <c r="A24" s="82"/>
+      <c r="B24" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="86"/>
-      <c r="D24" s="85"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="91" t="s">
+      <c r="C24" s="93"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="92"/>
-      <c r="H24" s="93"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="80"/>
       <c r="I24" s="8"/>
       <c r="J24" s="2"/>
       <c r="K24" s="3"/>
@@ -3841,18 +3850,18 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="77"/>
-      <c r="B25" s="88" t="s">
+      <c r="A25" s="82"/>
+      <c r="B25" s="89" t="s">
         <v>460</v>
       </c>
-      <c r="C25" s="86"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="91" t="s">
+      <c r="C25" s="93"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="G25" s="92"/>
-      <c r="H25" s="93"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="80"/>
       <c r="I25" s="8"/>
       <c r="J25" s="2"/>
       <c r="K25" s="3"/>
@@ -3873,18 +3882,18 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="78"/>
-      <c r="B26" s="91" t="s">
+      <c r="A26" s="84"/>
+      <c r="B26" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="92"/>
-      <c r="D26" s="93"/>
-      <c r="E26" s="99"/>
-      <c r="F26" s="91" t="s">
+      <c r="C26" s="79"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="78" t="s">
         <v>466</v>
       </c>
-      <c r="G26" s="92"/>
-      <c r="H26" s="93"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="80"/>
       <c r="I26" s="8"/>
       <c r="J26" s="2"/>
       <c r="K26" s="3"/>
@@ -3933,7 +3942,7 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="101" t="s">
+      <c r="A28" s="123" t="s">
         <v>70</v>
       </c>
       <c r="B28" s="64" t="s">
@@ -3945,7 +3954,7 @@
       <c r="D28" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="97" t="s">
+      <c r="E28" s="85" t="s">
         <v>13</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -3977,7 +3986,7 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="77"/>
+      <c r="A29" s="82"/>
       <c r="B29" s="64" t="s">
         <v>535</v>
       </c>
@@ -3987,7 +3996,7 @@
       <c r="D29" s="40" t="s">
         <v>438</v>
       </c>
-      <c r="E29" s="98"/>
+      <c r="E29" s="86"/>
       <c r="F29" s="8" t="s">
         <v>76</v>
       </c>
@@ -4017,7 +4026,7 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="77"/>
+      <c r="A30" s="82"/>
       <c r="B30" s="41" t="s">
         <v>79</v>
       </c>
@@ -4027,7 +4036,7 @@
       <c r="D30" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="98"/>
+      <c r="E30" s="86"/>
       <c r="F30" s="47" t="s">
         <v>82</v>
       </c>
@@ -4057,7 +4066,7 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="77"/>
+      <c r="A31" s="82"/>
       <c r="B31" s="45" t="s">
         <v>84</v>
       </c>
@@ -4067,7 +4076,7 @@
       <c r="D31" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="E31" s="98"/>
+      <c r="E31" s="86"/>
       <c r="F31" s="47" t="s">
         <v>87</v>
       </c>
@@ -4097,7 +4106,7 @@
       <c r="Z31" s="3"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="77"/>
+      <c r="A32" s="82"/>
       <c r="B32" s="41" t="s">
         <v>89</v>
       </c>
@@ -4107,7 +4116,7 @@
       <c r="D32" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="E32" s="98"/>
+      <c r="E32" s="86"/>
       <c r="F32" s="47" t="s">
         <v>92</v>
       </c>
@@ -4139,7 +4148,7 @@
       <c r="Z32" s="3"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="77"/>
+      <c r="A33" s="82"/>
       <c r="B33" s="58" t="s">
         <v>185</v>
       </c>
@@ -4149,7 +4158,7 @@
       <c r="D33" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="E33" s="98"/>
+      <c r="E33" s="86"/>
       <c r="F33" s="47" t="s">
         <v>97</v>
       </c>
@@ -4181,13 +4190,13 @@
       <c r="Z33" s="3"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="77"/>
+      <c r="A34" s="82"/>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
       <c r="D34" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="98"/>
+      <c r="E34" s="86"/>
       <c r="F34" s="47" t="s">
         <v>100</v>
       </c>
@@ -4219,7 +4228,7 @@
       <c r="Z34" s="3"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="77"/>
+      <c r="A35" s="82"/>
       <c r="B35" s="38"/>
       <c r="C35" s="40" t="s">
         <v>103</v>
@@ -4227,7 +4236,7 @@
       <c r="D35" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="E35" s="98"/>
+      <c r="E35" s="86"/>
       <c r="F35" s="65" t="s">
         <v>435</v>
       </c>
@@ -4259,7 +4268,7 @@
       <c r="Z35" s="3"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="77"/>
+      <c r="A36" s="82"/>
       <c r="B36" s="63" t="s">
         <v>106</v>
       </c>
@@ -4267,7 +4276,7 @@
       <c r="D36" s="40" t="s">
         <v>586</v>
       </c>
-      <c r="E36" s="98"/>
+      <c r="E36" s="86"/>
       <c r="F36" s="47" t="s">
         <v>107</v>
       </c>
@@ -4295,13 +4304,13 @@
       <c r="Z36" s="3"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="77"/>
+      <c r="A37" s="82"/>
       <c r="B37" s="40"/>
       <c r="C37" s="63" t="s">
         <v>536</v>
       </c>
       <c r="D37" s="40"/>
-      <c r="E37" s="98"/>
+      <c r="E37" s="86"/>
       <c r="F37" s="47" t="s">
         <v>109</v>
       </c>
@@ -4329,7 +4338,7 @@
       <c r="Z37" s="3"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="77"/>
+      <c r="A38" s="82"/>
       <c r="B38" s="40"/>
       <c r="C38" s="41" t="s">
         <v>111</v>
@@ -4337,7 +4346,7 @@
       <c r="D38" s="64" t="s">
         <v>537</v>
       </c>
-      <c r="E38" s="98"/>
+      <c r="E38" s="86"/>
       <c r="F38" s="66" t="s">
         <v>541</v>
       </c>
@@ -4367,7 +4376,7 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="77"/>
+      <c r="A39" s="82"/>
       <c r="B39" s="38"/>
       <c r="C39" s="73" t="s">
         <v>602</v>
@@ -4375,7 +4384,7 @@
       <c r="D39" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="E39" s="98"/>
+      <c r="E39" s="86"/>
       <c r="F39" s="66" t="s">
         <v>542</v>
       </c>
@@ -4403,12 +4412,12 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="77"/>
+      <c r="A40" s="82"/>
       <c r="B40" s="38"/>
       <c r="C40" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="E40" s="98"/>
+      <c r="E40" s="86"/>
       <c r="F40" s="48"/>
       <c r="G40" s="50" t="s">
         <v>117</v>
@@ -4434,13 +4443,13 @@
       <c r="Z40" s="3"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="77"/>
+      <c r="A41" s="82"/>
       <c r="B41" s="40"/>
       <c r="C41" s="41" t="s">
         <v>118</v>
       </c>
       <c r="D41" s="40"/>
-      <c r="E41" s="98"/>
+      <c r="E41" s="86"/>
       <c r="F41" s="48"/>
       <c r="G41" s="50"/>
       <c r="H41" s="50"/>
@@ -4464,14 +4473,14 @@
       <c r="Z41" s="3"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="77"/>
+      <c r="A42" s="82"/>
       <c r="B42" s="40"/>
       <c r="D42" s="40"/>
-      <c r="E42" s="98"/>
-      <c r="F42" s="102" t="s">
+      <c r="E42" s="86"/>
+      <c r="F42" s="120" t="s">
         <v>119</v>
       </c>
-      <c r="G42" s="85"/>
+      <c r="G42" s="77"/>
       <c r="H42" s="50"/>
       <c r="I42" s="48"/>
       <c r="J42" s="2"/>
@@ -4493,21 +4502,21 @@
       <c r="Z42" s="3"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="77"/>
+      <c r="A43" s="82"/>
       <c r="B43" s="40"/>
-      <c r="C43" s="82" t="s">
+      <c r="C43" s="91" t="s">
         <v>538</v>
       </c>
-      <c r="D43" s="83"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="102" t="s">
+      <c r="D43" s="92"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="120" t="s">
         <v>120</v>
       </c>
-      <c r="G43" s="85"/>
-      <c r="H43" s="82" t="s">
+      <c r="G43" s="77"/>
+      <c r="H43" s="91" t="s">
         <v>545</v>
       </c>
-      <c r="I43" s="83"/>
+      <c r="I43" s="92"/>
       <c r="J43" s="2"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
@@ -4527,21 +4536,21 @@
       <c r="Z43" s="3"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="77"/>
+      <c r="A44" s="82"/>
       <c r="B44" s="40"/>
-      <c r="C44" s="82" t="s">
+      <c r="C44" s="91" t="s">
         <v>539</v>
       </c>
-      <c r="D44" s="83"/>
-      <c r="E44" s="98"/>
-      <c r="F44" s="102" t="s">
+      <c r="D44" s="92"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="120" t="s">
         <v>121</v>
       </c>
-      <c r="G44" s="85"/>
-      <c r="H44" s="82" t="s">
+      <c r="G44" s="77"/>
+      <c r="H44" s="91" t="s">
         <v>546</v>
       </c>
-      <c r="I44" s="83"/>
+      <c r="I44" s="92"/>
       <c r="J44" s="2"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
@@ -4561,21 +4570,21 @@
       <c r="Z44" s="3"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="77"/>
+      <c r="A45" s="82"/>
       <c r="B45" s="40"/>
-      <c r="C45" s="82" t="s">
+      <c r="C45" s="91" t="s">
         <v>540</v>
       </c>
-      <c r="D45" s="82"/>
-      <c r="E45" s="98"/>
-      <c r="F45" s="84" t="s">
+      <c r="D45" s="91"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="94" t="s">
         <v>487</v>
       </c>
-      <c r="G45" s="85"/>
-      <c r="H45" s="84" t="s">
+      <c r="G45" s="77"/>
+      <c r="H45" s="94" t="s">
         <v>122</v>
       </c>
-      <c r="I45" s="85"/>
+      <c r="I45" s="77"/>
       <c r="J45" s="2"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
@@ -4595,21 +4604,21 @@
       <c r="Z45" s="3"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="77"/>
+      <c r="A46" s="82"/>
       <c r="B46" s="41"/>
-      <c r="C46" s="88" t="s">
+      <c r="C46" s="89" t="s">
         <v>486</v>
       </c>
-      <c r="D46" s="85"/>
-      <c r="E46" s="98"/>
-      <c r="F46" s="84" t="s">
+      <c r="D46" s="77"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="94" t="s">
         <v>123</v>
       </c>
-      <c r="G46" s="85"/>
-      <c r="H46" s="84" t="s">
+      <c r="G46" s="77"/>
+      <c r="H46" s="94" t="s">
         <v>495</v>
       </c>
-      <c r="I46" s="85"/>
+      <c r="I46" s="77"/>
       <c r="J46" s="2"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
@@ -4629,21 +4638,21 @@
       <c r="Z46" s="3"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="77"/>
+      <c r="A47" s="82"/>
       <c r="B47" s="41"/>
-      <c r="C47" s="88" t="s">
+      <c r="C47" s="89" t="s">
         <v>496</v>
       </c>
-      <c r="D47" s="85"/>
-      <c r="E47" s="98"/>
-      <c r="F47" s="94" t="s">
+      <c r="D47" s="77"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="98" t="s">
         <v>446</v>
       </c>
-      <c r="G47" s="85"/>
-      <c r="H47" s="94" t="s">
+      <c r="G47" s="77"/>
+      <c r="H47" s="98" t="s">
         <v>124</v>
       </c>
-      <c r="I47" s="85"/>
+      <c r="I47" s="77"/>
       <c r="J47" s="2"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
@@ -4663,21 +4672,21 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="77"/>
+      <c r="A48" s="82"/>
       <c r="B48" s="40"/>
-      <c r="C48" s="103" t="s">
+      <c r="C48" s="97" t="s">
         <v>125</v>
       </c>
-      <c r="D48" s="85"/>
-      <c r="E48" s="98"/>
-      <c r="F48" s="94" t="s">
+      <c r="D48" s="77"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="98" t="s">
         <v>447</v>
       </c>
-      <c r="G48" s="85"/>
-      <c r="H48" s="94" t="s">
+      <c r="G48" s="77"/>
+      <c r="H48" s="98" t="s">
         <v>516</v>
       </c>
-      <c r="I48" s="85"/>
+      <c r="I48" s="77"/>
       <c r="J48" s="2"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
@@ -4697,21 +4706,21 @@
       <c r="Z48" s="3"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="77"/>
+      <c r="A49" s="82"/>
       <c r="B49" s="40"/>
-      <c r="C49" s="103" t="s">
+      <c r="C49" s="97" t="s">
         <v>512</v>
       </c>
-      <c r="D49" s="85"/>
-      <c r="E49" s="98"/>
-      <c r="F49" s="84" t="s">
+      <c r="D49" s="77"/>
+      <c r="E49" s="86"/>
+      <c r="F49" s="94" t="s">
         <v>126</v>
       </c>
-      <c r="G49" s="85"/>
-      <c r="H49" s="84" t="s">
+      <c r="G49" s="77"/>
+      <c r="H49" s="94" t="s">
         <v>127</v>
       </c>
-      <c r="I49" s="85"/>
+      <c r="I49" s="77"/>
       <c r="J49" s="2"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
@@ -4731,21 +4740,21 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="77"/>
+      <c r="A50" s="82"/>
       <c r="B50" s="40"/>
-      <c r="C50" s="88" t="s">
+      <c r="C50" s="89" t="s">
         <v>128</v>
       </c>
-      <c r="D50" s="85"/>
-      <c r="E50" s="98"/>
-      <c r="F50" s="84" t="s">
+      <c r="D50" s="77"/>
+      <c r="E50" s="86"/>
+      <c r="F50" s="94" t="s">
         <v>129</v>
       </c>
-      <c r="G50" s="85"/>
-      <c r="H50" s="84" t="s">
+      <c r="G50" s="77"/>
+      <c r="H50" s="94" t="s">
         <v>130</v>
       </c>
-      <c r="I50" s="85"/>
+      <c r="I50" s="77"/>
       <c r="J50" s="2"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
@@ -4765,19 +4774,19 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="77"/>
+      <c r="A51" s="82"/>
       <c r="B51" s="8"/>
-      <c r="C51" s="91" t="s">
+      <c r="C51" s="78" t="s">
         <v>131</v>
       </c>
-      <c r="D51" s="93"/>
-      <c r="E51" s="98"/>
+      <c r="D51" s="80"/>
+      <c r="E51" s="86"/>
       <c r="F51" s="47"/>
       <c r="G51" s="50"/>
-      <c r="H51" s="104" t="s">
+      <c r="H51" s="124" t="s">
         <v>591</v>
       </c>
-      <c r="I51" s="105"/>
+      <c r="I51" s="125"/>
       <c r="J51" s="2"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
@@ -4797,18 +4806,18 @@
       <c r="Z51" s="3"/>
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="77"/>
-      <c r="B52" s="91" t="s">
+      <c r="A52" s="82"/>
+      <c r="B52" s="78" t="s">
         <v>461</v>
       </c>
-      <c r="C52" s="92"/>
-      <c r="D52" s="93"/>
-      <c r="E52" s="98"/>
-      <c r="F52" s="84" t="s">
+      <c r="C52" s="79"/>
+      <c r="D52" s="80"/>
+      <c r="E52" s="86"/>
+      <c r="F52" s="94" t="s">
         <v>132</v>
       </c>
-      <c r="G52" s="86"/>
-      <c r="H52" s="85"/>
+      <c r="G52" s="93"/>
+      <c r="H52" s="77"/>
       <c r="I52" s="50"/>
       <c r="J52" s="2"/>
       <c r="K52" s="3"/>
@@ -4829,18 +4838,18 @@
       <c r="Z52" s="3"/>
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="77"/>
-      <c r="B53" s="91" t="s">
+      <c r="A53" s="82"/>
+      <c r="B53" s="78" t="s">
         <v>478</v>
       </c>
-      <c r="C53" s="92"/>
-      <c r="D53" s="93"/>
-      <c r="E53" s="98"/>
-      <c r="F53" s="91" t="s">
+      <c r="C53" s="79"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="86"/>
+      <c r="F53" s="78" t="s">
         <v>479</v>
       </c>
-      <c r="G53" s="92"/>
-      <c r="H53" s="93"/>
+      <c r="G53" s="79"/>
+      <c r="H53" s="80"/>
       <c r="I53" s="9"/>
       <c r="J53" s="2"/>
       <c r="K53" s="3"/>
@@ -4861,18 +4870,18 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="78"/>
-      <c r="B54" s="91" t="s">
+      <c r="A54" s="84"/>
+      <c r="B54" s="78" t="s">
         <v>133</v>
       </c>
-      <c r="C54" s="92"/>
-      <c r="D54" s="93"/>
-      <c r="E54" s="99"/>
-      <c r="F54" s="91" t="s">
+      <c r="C54" s="79"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="88"/>
+      <c r="F54" s="78" t="s">
         <v>467</v>
       </c>
-      <c r="G54" s="92"/>
-      <c r="H54" s="93"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="80"/>
       <c r="I54" s="9"/>
       <c r="J54" s="2"/>
       <c r="K54" s="3"/>
@@ -4921,7 +4930,7 @@
       <c r="Z55" s="3"/>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="129" t="s">
+      <c r="A56" s="81" t="s">
         <v>134</v>
       </c>
       <c r="B56" s="41" t="s">
@@ -4933,7 +4942,7 @@
       <c r="D56" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="E56" s="97" t="s">
+      <c r="E56" s="85" t="s">
         <v>13</v>
       </c>
       <c r="F56" s="63" t="s">
@@ -4965,7 +4974,7 @@
       <c r="Z56" s="3"/>
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="77"/>
+      <c r="A57" s="82"/>
       <c r="B57" s="41" t="s">
         <v>136</v>
       </c>
@@ -4975,7 +4984,7 @@
       <c r="D57" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="E57" s="98"/>
+      <c r="E57" s="86"/>
       <c r="F57" s="63" t="s">
         <v>138</v>
       </c>
@@ -5005,7 +5014,7 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="77"/>
+      <c r="A58" s="82"/>
       <c r="B58" s="40" t="s">
         <v>454</v>
       </c>
@@ -5015,7 +5024,7 @@
       <c r="D58" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="E58" s="98"/>
+      <c r="E58" s="86"/>
       <c r="F58" s="63" t="s">
         <v>24</v>
       </c>
@@ -5045,14 +5054,14 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="77"/>
+      <c r="A59" s="82"/>
       <c r="B59" s="40" t="s">
         <v>510</v>
       </c>
       <c r="C59" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="E59" s="98"/>
+      <c r="E59" s="86"/>
       <c r="F59" s="40" t="s">
         <v>87</v>
       </c>
@@ -5081,7 +5090,7 @@
       <c r="Z59" s="3"/>
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="77"/>
+      <c r="A60" s="82"/>
       <c r="B60" s="73" t="s">
         <v>607</v>
       </c>
@@ -5091,7 +5100,7 @@
       <c r="D60" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="E60" s="98"/>
+      <c r="E60" s="86"/>
       <c r="F60" s="63" t="s">
         <v>93</v>
       </c>
@@ -5121,7 +5130,7 @@
       <c r="Z60" s="3"/>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="77"/>
+      <c r="A61" s="82"/>
       <c r="B61" s="40"/>
       <c r="C61" s="40" t="s">
         <v>143</v>
@@ -5129,7 +5138,7 @@
       <c r="D61" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="E61" s="98"/>
+      <c r="E61" s="86"/>
       <c r="F61" s="63" t="s">
         <v>544</v>
       </c>
@@ -5159,7 +5168,7 @@
       <c r="Z61" s="3"/>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="77"/>
+      <c r="A62" s="82"/>
       <c r="B62" s="40"/>
       <c r="C62" s="40" t="s">
         <v>611</v>
@@ -5167,7 +5176,7 @@
       <c r="D62" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="E62" s="98"/>
+      <c r="E62" s="86"/>
       <c r="F62" s="63" t="s">
         <v>101</v>
       </c>
@@ -5197,7 +5206,7 @@
       <c r="Z62" s="3"/>
     </row>
     <row r="63" spans="1:26" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="77"/>
+      <c r="A63" s="82"/>
       <c r="B63" s="40"/>
       <c r="C63" s="40" t="s">
         <v>443</v>
@@ -5205,7 +5214,7 @@
       <c r="D63" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="E63" s="98"/>
+      <c r="E63" s="86"/>
       <c r="F63" s="63" t="s">
         <v>145</v>
       </c>
@@ -5235,7 +5244,7 @@
       <c r="Z63" s="3"/>
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="77"/>
+      <c r="A64" s="82"/>
       <c r="B64" s="40"/>
       <c r="C64" s="41" t="s">
         <v>147</v>
@@ -5243,7 +5252,7 @@
       <c r="D64" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="E64" s="98"/>
+      <c r="E64" s="86"/>
       <c r="F64" s="63" t="s">
         <v>543</v>
       </c>
@@ -5273,7 +5282,7 @@
       <c r="Z64" s="3"/>
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="77"/>
+      <c r="A65" s="82"/>
       <c r="B65" s="40"/>
       <c r="C65" s="64" t="s">
         <v>548</v>
@@ -5281,7 +5290,7 @@
       <c r="D65" s="64" t="s">
         <v>549</v>
       </c>
-      <c r="E65" s="98"/>
+      <c r="E65" s="86"/>
       <c r="G65" s="63" t="s">
         <v>555</v>
       </c>
@@ -5310,7 +5319,7 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="77"/>
+      <c r="A66" s="82"/>
       <c r="B66" s="40"/>
       <c r="C66" s="40" t="s">
         <v>149</v>
@@ -5318,7 +5327,7 @@
       <c r="D66" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="E66" s="98"/>
+      <c r="E66" s="86"/>
       <c r="F66" s="40" t="s">
         <v>151</v>
       </c>
@@ -5350,13 +5359,13 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="77"/>
+      <c r="A67" s="82"/>
       <c r="B67" s="40"/>
       <c r="C67" s="38"/>
       <c r="D67" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E67" s="98"/>
+      <c r="E67" s="86"/>
       <c r="F67" s="64" t="s">
         <v>553</v>
       </c>
@@ -5384,13 +5393,13 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="77"/>
+      <c r="A68" s="82"/>
       <c r="B68" s="40"/>
       <c r="C68" s="38"/>
       <c r="D68" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="E68" s="98"/>
+      <c r="E68" s="86"/>
       <c r="F68" s="64" t="s">
         <v>554</v>
       </c>
@@ -5418,13 +5427,13 @@
       <c r="Z68" s="3"/>
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="77"/>
+      <c r="A69" s="82"/>
       <c r="B69" s="38"/>
       <c r="C69" s="38"/>
       <c r="D69" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="E69" s="98"/>
+      <c r="E69" s="86"/>
       <c r="G69" s="38"/>
       <c r="H69" s="40"/>
       <c r="I69" s="41"/>
@@ -5447,13 +5456,13 @@
       <c r="Z69" s="3"/>
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="77"/>
+      <c r="A70" s="82"/>
       <c r="B70" s="40"/>
       <c r="C70" s="38"/>
       <c r="D70" s="73" t="s">
         <v>603</v>
       </c>
-      <c r="E70" s="98"/>
+      <c r="E70" s="86"/>
       <c r="F70" s="38"/>
       <c r="G70" s="38"/>
       <c r="H70" s="40"/>
@@ -5477,19 +5486,19 @@
       <c r="Z70" s="3"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="77"/>
-      <c r="B71" s="88" t="s">
+      <c r="A71" s="82"/>
+      <c r="B71" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="C71" s="85"/>
+      <c r="C71" s="77"/>
       <c r="D71" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="E71" s="98"/>
-      <c r="F71" s="132" t="s">
+      <c r="E71" s="86"/>
+      <c r="F71" s="90" t="s">
         <v>592</v>
       </c>
-      <c r="G71" s="85"/>
+      <c r="G71" s="77"/>
       <c r="H71" s="40"/>
       <c r="I71" s="41"/>
       <c r="J71" s="2"/>
@@ -5511,13 +5520,13 @@
       <c r="Z71" s="3"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="130"/>
+      <c r="A72" s="83"/>
       <c r="B72" s="54"/>
       <c r="C72" s="60"/>
       <c r="D72" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E72" s="131"/>
+      <c r="E72" s="87"/>
       <c r="F72" s="61"/>
       <c r="G72" s="59"/>
       <c r="H72" s="54"/>
@@ -5541,21 +5550,21 @@
       <c r="Z72" s="3"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="77"/>
+      <c r="A73" s="82"/>
       <c r="B73" s="40"/>
-      <c r="C73" s="82" t="s">
+      <c r="C73" s="91" t="s">
         <v>550</v>
       </c>
-      <c r="D73" s="83"/>
-      <c r="E73" s="98"/>
-      <c r="F73" s="126" t="s">
+      <c r="D73" s="92"/>
+      <c r="E73" s="86"/>
+      <c r="F73" s="95" t="s">
         <v>560</v>
       </c>
-      <c r="G73" s="127"/>
-      <c r="H73" s="126" t="s">
+      <c r="G73" s="96"/>
+      <c r="H73" s="95" t="s">
         <v>561</v>
       </c>
-      <c r="I73" s="127"/>
+      <c r="I73" s="96"/>
       <c r="J73" s="2"/>
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
@@ -5575,21 +5584,21 @@
       <c r="Z73" s="3"/>
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="77"/>
+      <c r="A74" s="82"/>
       <c r="B74" s="40"/>
-      <c r="C74" s="82" t="s">
+      <c r="C74" s="91" t="s">
         <v>551</v>
       </c>
-      <c r="D74" s="83"/>
-      <c r="E74" s="98"/>
-      <c r="F74" s="82" t="s">
+      <c r="D74" s="92"/>
+      <c r="E74" s="86"/>
+      <c r="F74" s="91" t="s">
         <v>562</v>
       </c>
-      <c r="G74" s="83"/>
-      <c r="H74" s="82" t="s">
+      <c r="G74" s="92"/>
+      <c r="H74" s="91" t="s">
         <v>563</v>
       </c>
-      <c r="I74" s="83"/>
+      <c r="I74" s="92"/>
       <c r="J74" s="2"/>
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
@@ -5609,21 +5618,21 @@
       <c r="Z74" s="3"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="77"/>
+      <c r="A75" s="82"/>
       <c r="B75" s="41"/>
-      <c r="C75" s="88" t="s">
+      <c r="C75" s="89" t="s">
         <v>488</v>
       </c>
-      <c r="D75" s="85"/>
-      <c r="E75" s="98"/>
-      <c r="F75" s="88" t="s">
+      <c r="D75" s="77"/>
+      <c r="E75" s="86"/>
+      <c r="F75" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="G75" s="85"/>
-      <c r="H75" s="88" t="s">
+      <c r="G75" s="77"/>
+      <c r="H75" s="89" t="s">
         <v>596</v>
       </c>
-      <c r="I75" s="85"/>
+      <c r="I75" s="77"/>
       <c r="J75" s="2"/>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
@@ -5643,21 +5652,21 @@
       <c r="Z75" s="3"/>
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="77"/>
+      <c r="A76" s="82"/>
       <c r="B76" s="41"/>
-      <c r="C76" s="88" t="s">
+      <c r="C76" s="89" t="s">
         <v>158</v>
       </c>
-      <c r="D76" s="85"/>
-      <c r="E76" s="98"/>
-      <c r="F76" s="88" t="s">
+      <c r="D76" s="77"/>
+      <c r="E76" s="86"/>
+      <c r="F76" s="89" t="s">
         <v>489</v>
       </c>
-      <c r="G76" s="85"/>
-      <c r="H76" s="88" t="s">
+      <c r="G76" s="77"/>
+      <c r="H76" s="89" t="s">
         <v>159</v>
       </c>
-      <c r="I76" s="85"/>
+      <c r="I76" s="77"/>
       <c r="J76" s="2"/>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
@@ -5677,21 +5686,21 @@
       <c r="Z76" s="3"/>
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="77"/>
+      <c r="A77" s="82"/>
       <c r="B77" s="40"/>
-      <c r="C77" s="103" t="s">
+      <c r="C77" s="97" t="s">
         <v>160</v>
       </c>
-      <c r="D77" s="85"/>
-      <c r="E77" s="98"/>
-      <c r="F77" s="103" t="s">
+      <c r="D77" s="77"/>
+      <c r="E77" s="86"/>
+      <c r="F77" s="97" t="s">
         <v>161</v>
       </c>
-      <c r="G77" s="85"/>
-      <c r="H77" s="103" t="s">
+      <c r="G77" s="77"/>
+      <c r="H77" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="I77" s="85"/>
+      <c r="I77" s="77"/>
       <c r="J77" s="2"/>
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
@@ -5711,21 +5720,21 @@
       <c r="Z77" s="3"/>
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="77"/>
+      <c r="A78" s="82"/>
       <c r="B78" s="40"/>
-      <c r="C78" s="103" t="s">
+      <c r="C78" s="97" t="s">
         <v>448</v>
       </c>
-      <c r="D78" s="85"/>
-      <c r="E78" s="98"/>
-      <c r="F78" s="103" t="s">
+      <c r="D78" s="77"/>
+      <c r="E78" s="86"/>
+      <c r="F78" s="97" t="s">
         <v>432</v>
       </c>
-      <c r="G78" s="85"/>
-      <c r="H78" s="103" t="s">
+      <c r="G78" s="77"/>
+      <c r="H78" s="97" t="s">
         <v>505</v>
       </c>
-      <c r="I78" s="85"/>
+      <c r="I78" s="77"/>
       <c r="J78" s="2"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
@@ -5745,21 +5754,21 @@
       <c r="Z78" s="3"/>
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="77"/>
+      <c r="A79" s="82"/>
       <c r="B79" s="40"/>
-      <c r="C79" s="88" t="s">
+      <c r="C79" s="89" t="s">
         <v>163</v>
       </c>
-      <c r="D79" s="85"/>
-      <c r="E79" s="98"/>
-      <c r="F79" s="88" t="s">
+      <c r="D79" s="77"/>
+      <c r="E79" s="86"/>
+      <c r="F79" s="89" t="s">
         <v>164</v>
       </c>
-      <c r="G79" s="85"/>
-      <c r="H79" s="88" t="s">
+      <c r="G79" s="77"/>
+      <c r="H79" s="89" t="s">
         <v>456</v>
       </c>
-      <c r="I79" s="85"/>
+      <c r="I79" s="77"/>
       <c r="J79" s="2"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
@@ -5779,21 +5788,21 @@
       <c r="Z79" s="3"/>
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="77"/>
+      <c r="A80" s="82"/>
       <c r="B80" s="40"/>
-      <c r="C80" s="88" t="s">
+      <c r="C80" s="89" t="s">
         <v>165</v>
       </c>
-      <c r="D80" s="85"/>
-      <c r="E80" s="98"/>
-      <c r="F80" s="88" t="s">
+      <c r="D80" s="77"/>
+      <c r="E80" s="86"/>
+      <c r="F80" s="89" t="s">
         <v>455</v>
       </c>
-      <c r="G80" s="85"/>
-      <c r="H80" s="88" t="s">
+      <c r="G80" s="77"/>
+      <c r="H80" s="89" t="s">
         <v>166</v>
       </c>
-      <c r="I80" s="85"/>
+      <c r="I80" s="77"/>
       <c r="J80" s="2"/>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
@@ -5813,18 +5822,18 @@
       <c r="Z80" s="3"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="77"/>
-      <c r="B81" s="91" t="s">
+      <c r="A81" s="82"/>
+      <c r="B81" s="78" t="s">
         <v>167</v>
       </c>
-      <c r="C81" s="92"/>
-      <c r="D81" s="93"/>
-      <c r="E81" s="98"/>
-      <c r="F81" s="88" t="s">
+      <c r="C81" s="79"/>
+      <c r="D81" s="80"/>
+      <c r="E81" s="86"/>
+      <c r="F81" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="G81" s="86"/>
-      <c r="H81" s="85"/>
+      <c r="G81" s="93"/>
+      <c r="H81" s="77"/>
       <c r="I81" s="41"/>
       <c r="J81" s="2"/>
       <c r="K81" s="3"/>
@@ -5845,18 +5854,18 @@
       <c r="Z81" s="3"/>
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="77"/>
-      <c r="B82" s="91" t="s">
+      <c r="A82" s="82"/>
+      <c r="B82" s="78" t="s">
         <v>169</v>
       </c>
-      <c r="C82" s="92"/>
-      <c r="D82" s="93"/>
-      <c r="E82" s="98"/>
-      <c r="F82" s="91" t="s">
+      <c r="C82" s="79"/>
+      <c r="D82" s="80"/>
+      <c r="E82" s="86"/>
+      <c r="F82" s="78" t="s">
         <v>468</v>
       </c>
-      <c r="G82" s="92"/>
-      <c r="H82" s="93"/>
+      <c r="G82" s="79"/>
+      <c r="H82" s="80"/>
       <c r="I82" s="9"/>
       <c r="J82" s="2"/>
       <c r="K82" s="3"/>
@@ -5877,18 +5886,18 @@
       <c r="Z82" s="3"/>
     </row>
     <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="78"/>
-      <c r="B83" s="91" t="s">
+      <c r="A83" s="84"/>
+      <c r="B83" s="78" t="s">
         <v>170</v>
       </c>
-      <c r="C83" s="92"/>
-      <c r="D83" s="93"/>
-      <c r="E83" s="99"/>
-      <c r="F83" s="91" t="s">
+      <c r="C83" s="79"/>
+      <c r="D83" s="80"/>
+      <c r="E83" s="88"/>
+      <c r="F83" s="78" t="s">
         <v>469</v>
       </c>
-      <c r="G83" s="92"/>
-      <c r="H83" s="93"/>
+      <c r="G83" s="79"/>
+      <c r="H83" s="80"/>
       <c r="I83" s="9"/>
       <c r="J83" s="2"/>
       <c r="K83" s="3"/>
@@ -5937,7 +5946,7 @@
       <c r="Z84" s="3"/>
     </row>
     <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="121" t="s">
+      <c r="A85" s="104" t="s">
         <v>171</v>
       </c>
       <c r="B85" s="9" t="s">
@@ -5949,7 +5958,7 @@
       <c r="D85" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E85" s="97" t="s">
+      <c r="E85" s="85" t="s">
         <v>13</v>
       </c>
       <c r="F85" s="63" t="s">
@@ -5983,7 +5992,7 @@
       <c r="Z85" s="3"/>
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="77"/>
+      <c r="A86" s="82"/>
       <c r="B86" s="9" t="s">
         <v>174</v>
       </c>
@@ -5993,7 +6002,7 @@
       <c r="D86" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="E86" s="98"/>
+      <c r="E86" s="86"/>
       <c r="F86" s="63" t="s">
         <v>522</v>
       </c>
@@ -6025,7 +6034,7 @@
       <c r="Z86" s="3"/>
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="77"/>
+      <c r="A87" s="82"/>
       <c r="B87" s="8" t="s">
         <v>178</v>
       </c>
@@ -6035,7 +6044,7 @@
       <c r="D87" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E87" s="98"/>
+      <c r="E87" s="86"/>
       <c r="F87" s="65" t="s">
         <v>523</v>
       </c>
@@ -6067,7 +6076,7 @@
       <c r="Z87" s="3"/>
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="77"/>
+      <c r="A88" s="82"/>
       <c r="B88" s="40" t="s">
         <v>590</v>
       </c>
@@ -6075,7 +6084,7 @@
       <c r="D88" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="E88" s="98"/>
+      <c r="E88" s="86"/>
       <c r="F88" s="65" t="s">
         <v>26</v>
       </c>
@@ -6107,7 +6116,7 @@
       <c r="Z88" s="3"/>
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="77"/>
+      <c r="A89" s="82"/>
       <c r="B89" s="38"/>
       <c r="C89" s="47" t="s">
         <v>589</v>
@@ -6115,15 +6124,12 @@
       <c r="D89" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="E89" s="98"/>
+      <c r="E89" s="86"/>
       <c r="F89" s="65" t="s">
         <v>547</v>
       </c>
       <c r="G89" s="47" t="s">
         <v>32</v>
-      </c>
-      <c r="H89" s="47" t="s">
-        <v>182</v>
       </c>
       <c r="I89" s="47" t="s">
         <v>511</v>
@@ -6147,7 +6153,7 @@
       <c r="Z89" s="3"/>
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="77"/>
+      <c r="A90" s="82"/>
       <c r="B90" s="40" t="s">
         <v>99</v>
       </c>
@@ -6157,7 +6163,7 @@
       <c r="D90" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E90" s="98"/>
+      <c r="E90" s="86"/>
       <c r="F90" s="65" t="s">
         <v>524</v>
       </c>
@@ -6186,14 +6192,14 @@
       <c r="Z90" s="3"/>
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="77"/>
+      <c r="A91" s="82"/>
       <c r="B91" s="40" t="s">
         <v>184</v>
       </c>
       <c r="D91" s="40" t="s">
         <v>185</v>
       </c>
-      <c r="E91" s="98"/>
+      <c r="E91" s="86"/>
       <c r="F91" s="65" t="s">
         <v>38</v>
       </c>
@@ -6223,14 +6229,14 @@
       <c r="Z91" s="3"/>
     </row>
     <row r="92" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="77"/>
+      <c r="A92" s="82"/>
       <c r="C92" s="40" t="s">
         <v>90</v>
       </c>
       <c r="D92" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="E92" s="98"/>
+      <c r="E92" s="86"/>
       <c r="F92" s="47" t="s">
         <v>107</v>
       </c>
@@ -6257,7 +6263,7 @@
       <c r="Z92" s="3"/>
     </row>
     <row r="93" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="77"/>
+      <c r="A93" s="82"/>
       <c r="B93" s="38"/>
       <c r="C93" s="40" t="s">
         <v>188</v>
@@ -6265,7 +6271,7 @@
       <c r="D93" s="50" t="s">
         <v>612</v>
       </c>
-      <c r="E93" s="98"/>
+      <c r="E93" s="86"/>
       <c r="F93" s="65" t="s">
         <v>436</v>
       </c>
@@ -6295,13 +6301,13 @@
       <c r="Z93" s="3"/>
     </row>
     <row r="94" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="77"/>
+      <c r="A94" s="82"/>
       <c r="B94" s="38"/>
       <c r="C94" s="42"/>
       <c r="D94" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="E94" s="98"/>
+      <c r="E94" s="86"/>
       <c r="F94" s="47" t="s">
         <v>520</v>
       </c>
@@ -6327,7 +6333,7 @@
       <c r="Z94" s="3"/>
     </row>
     <row r="95" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="77"/>
+      <c r="A95" s="82"/>
       <c r="B95" s="63" t="s">
         <v>564</v>
       </c>
@@ -6337,7 +6343,7 @@
       <c r="D95" s="41" t="s">
         <v>191</v>
       </c>
-      <c r="E95" s="98"/>
+      <c r="E95" s="86"/>
       <c r="F95" s="47" t="s">
         <v>192</v>
       </c>
@@ -6367,15 +6373,15 @@
       <c r="Z95" s="3"/>
     </row>
     <row r="96" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="77"/>
-      <c r="B96" s="128" t="s">
+      <c r="A96" s="82"/>
+      <c r="B96" s="76" t="s">
         <v>593</v>
       </c>
-      <c r="C96" s="85"/>
+      <c r="C96" s="77"/>
       <c r="D96" s="63" t="s">
         <v>566</v>
       </c>
-      <c r="E96" s="98"/>
+      <c r="E96" s="86"/>
       <c r="F96" s="47" t="s">
         <v>194</v>
       </c>
@@ -6400,7 +6406,7 @@
       <c r="Z96" s="3"/>
     </row>
     <row r="97" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="77"/>
+      <c r="A97" s="82"/>
       <c r="B97" s="38"/>
       <c r="C97" s="40" t="s">
         <v>439</v>
@@ -6408,7 +6414,7 @@
       <c r="D97" s="63" t="s">
         <v>567</v>
       </c>
-      <c r="E97" s="98"/>
+      <c r="E97" s="86"/>
       <c r="F97" s="47"/>
       <c r="G97" s="48"/>
       <c r="H97" s="52" t="s">
@@ -6434,21 +6440,21 @@
       <c r="Z97" s="3"/>
     </row>
     <row r="98" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="77"/>
+      <c r="A98" s="82"/>
       <c r="B98" s="38"/>
-      <c r="C98" s="82" t="s">
+      <c r="C98" s="91" t="s">
         <v>568</v>
       </c>
-      <c r="D98" s="83"/>
-      <c r="E98" s="98"/>
-      <c r="F98" s="84" t="s">
+      <c r="D98" s="92"/>
+      <c r="E98" s="86"/>
+      <c r="F98" s="94" t="s">
         <v>196</v>
       </c>
-      <c r="G98" s="85"/>
-      <c r="H98" s="82" t="s">
+      <c r="G98" s="77"/>
+      <c r="H98" s="91" t="s">
         <v>574</v>
       </c>
-      <c r="I98" s="123"/>
+      <c r="I98" s="106"/>
       <c r="J98" s="2" t="s">
         <v>197</v>
       </c>
@@ -6470,21 +6476,21 @@
       <c r="Z98" s="3"/>
     </row>
     <row r="99" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="77"/>
+      <c r="A99" s="82"/>
       <c r="B99" s="40"/>
-      <c r="C99" s="82" t="s">
+      <c r="C99" s="91" t="s">
         <v>569</v>
       </c>
-      <c r="D99" s="83"/>
-      <c r="E99" s="98"/>
-      <c r="F99" s="82" t="s">
+      <c r="D99" s="92"/>
+      <c r="E99" s="86"/>
+      <c r="F99" s="91" t="s">
         <v>572</v>
       </c>
-      <c r="G99" s="83"/>
-      <c r="H99" s="82" t="s">
+      <c r="G99" s="92"/>
+      <c r="H99" s="91" t="s">
         <v>575</v>
       </c>
-      <c r="I99" s="83"/>
+      <c r="I99" s="92"/>
       <c r="J99" s="2"/>
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
@@ -6504,21 +6510,21 @@
       <c r="Z99" s="3"/>
     </row>
     <row r="100" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="77"/>
+      <c r="A100" s="82"/>
       <c r="B100" s="41"/>
-      <c r="C100" s="88" t="s">
+      <c r="C100" s="89" t="s">
         <v>198</v>
       </c>
-      <c r="D100" s="85"/>
-      <c r="E100" s="98"/>
-      <c r="F100" s="82" t="s">
+      <c r="D100" s="77"/>
+      <c r="E100" s="86"/>
+      <c r="F100" s="91" t="s">
         <v>573</v>
       </c>
-      <c r="G100" s="83"/>
-      <c r="H100" s="84" t="s">
+      <c r="G100" s="92"/>
+      <c r="H100" s="94" t="s">
         <v>490</v>
       </c>
-      <c r="I100" s="85"/>
+      <c r="I100" s="77"/>
       <c r="J100" s="2"/>
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
@@ -6538,21 +6544,21 @@
       <c r="Z100" s="3"/>
     </row>
     <row r="101" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="77"/>
+      <c r="A101" s="82"/>
       <c r="B101" s="41"/>
-      <c r="C101" s="88" t="s">
+      <c r="C101" s="89" t="s">
         <v>199</v>
       </c>
-      <c r="D101" s="85"/>
-      <c r="E101" s="98"/>
-      <c r="F101" s="84" t="s">
+      <c r="D101" s="77"/>
+      <c r="E101" s="86"/>
+      <c r="F101" s="94" t="s">
         <v>499</v>
       </c>
-      <c r="G101" s="85"/>
-      <c r="H101" s="84" t="s">
+      <c r="G101" s="77"/>
+      <c r="H101" s="94" t="s">
         <v>597</v>
       </c>
-      <c r="I101" s="85"/>
+      <c r="I101" s="77"/>
       <c r="J101" s="2"/>
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
@@ -6572,21 +6578,21 @@
       <c r="Z101" s="3"/>
     </row>
     <row r="102" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="77"/>
+      <c r="A102" s="82"/>
       <c r="B102" s="40"/>
-      <c r="C102" s="103" t="s">
+      <c r="C102" s="97" t="s">
         <v>426</v>
       </c>
-      <c r="D102" s="85"/>
-      <c r="E102" s="98"/>
-      <c r="F102" s="84" t="s">
+      <c r="D102" s="77"/>
+      <c r="E102" s="86"/>
+      <c r="F102" s="94" t="s">
         <v>200</v>
       </c>
-      <c r="G102" s="85"/>
-      <c r="H102" s="94" t="s">
+      <c r="G102" s="77"/>
+      <c r="H102" s="98" t="s">
         <v>507</v>
       </c>
-      <c r="I102" s="85"/>
+      <c r="I102" s="77"/>
       <c r="J102" s="2"/>
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
@@ -6606,17 +6612,17 @@
       <c r="Z102" s="3"/>
     </row>
     <row r="103" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="77"/>
+      <c r="A103" s="82"/>
       <c r="B103" s="40"/>
-      <c r="E103" s="98"/>
-      <c r="F103" s="84" t="s">
+      <c r="E103" s="86"/>
+      <c r="F103" s="94" t="s">
         <v>482</v>
       </c>
-      <c r="G103" s="85"/>
-      <c r="H103" s="117" t="s">
+      <c r="G103" s="77"/>
+      <c r="H103" s="101" t="s">
         <v>201</v>
       </c>
-      <c r="I103" s="85"/>
+      <c r="I103" s="77"/>
       <c r="J103" s="2"/>
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
@@ -6636,18 +6642,18 @@
       <c r="Z103" s="3"/>
     </row>
     <row r="104" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="77"/>
+      <c r="A104" s="82"/>
       <c r="B104" s="54"/>
       <c r="C104" s="56"/>
-      <c r="E104" s="122"/>
-      <c r="F104" s="94" t="s">
+      <c r="E104" s="105"/>
+      <c r="F104" s="98" t="s">
         <v>449</v>
       </c>
-      <c r="G104" s="85"/>
-      <c r="H104" s="84" t="s">
+      <c r="G104" s="77"/>
+      <c r="H104" s="94" t="s">
         <v>202</v>
       </c>
-      <c r="I104" s="85"/>
+      <c r="I104" s="77"/>
       <c r="J104" s="2"/>
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
@@ -6667,21 +6673,21 @@
       <c r="Z104" s="3"/>
     </row>
     <row r="105" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="77"/>
-      <c r="B105" s="124" t="s">
+      <c r="A105" s="82"/>
+      <c r="B105" s="99" t="s">
         <v>429</v>
       </c>
-      <c r="C105" s="125"/>
+      <c r="C105" s="100"/>
       <c r="D105" s="57"/>
-      <c r="E105" s="122"/>
-      <c r="F105" s="94" t="s">
+      <c r="E105" s="105"/>
+      <c r="F105" s="98" t="s">
         <v>431</v>
       </c>
-      <c r="G105" s="85"/>
-      <c r="H105" s="84" t="s">
+      <c r="G105" s="77"/>
+      <c r="H105" s="94" t="s">
         <v>203</v>
       </c>
-      <c r="I105" s="85"/>
+      <c r="I105" s="77"/>
       <c r="J105" s="2"/>
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
@@ -6701,15 +6707,15 @@
       <c r="Z105" s="3"/>
     </row>
     <row r="106" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="77"/>
+      <c r="A106" s="82"/>
       <c r="B106" s="55"/>
       <c r="C106" s="57"/>
       <c r="D106" s="57"/>
-      <c r="E106" s="122"/>
-      <c r="F106" s="84" t="s">
+      <c r="E106" s="105"/>
+      <c r="F106" s="94" t="s">
         <v>457</v>
       </c>
-      <c r="G106" s="85"/>
+      <c r="G106" s="77"/>
       <c r="H106" s="51"/>
       <c r="I106" s="51"/>
       <c r="J106" s="2"/>
@@ -6731,18 +6737,18 @@
       <c r="Z106" s="3"/>
     </row>
     <row r="107" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="77"/>
-      <c r="B107" s="91" t="s">
+      <c r="A107" s="82"/>
+      <c r="B107" s="78" t="s">
         <v>204</v>
       </c>
-      <c r="C107" s="119"/>
-      <c r="D107" s="120"/>
-      <c r="E107" s="98"/>
-      <c r="F107" s="84" t="s">
+      <c r="C107" s="102"/>
+      <c r="D107" s="103"/>
+      <c r="E107" s="86"/>
+      <c r="F107" s="94" t="s">
         <v>470</v>
       </c>
-      <c r="G107" s="86"/>
-      <c r="H107" s="85"/>
+      <c r="G107" s="93"/>
+      <c r="H107" s="77"/>
       <c r="I107" s="50"/>
       <c r="J107" s="2"/>
       <c r="K107" s="3"/>
@@ -6763,18 +6769,18 @@
       <c r="Z107" s="3"/>
     </row>
     <row r="108" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="77"/>
-      <c r="B108" s="91" t="s">
+      <c r="A108" s="82"/>
+      <c r="B108" s="78" t="s">
         <v>462</v>
       </c>
-      <c r="C108" s="92"/>
-      <c r="D108" s="93"/>
-      <c r="E108" s="98"/>
-      <c r="F108" s="91" t="s">
+      <c r="C108" s="79"/>
+      <c r="D108" s="80"/>
+      <c r="E108" s="86"/>
+      <c r="F108" s="78" t="s">
         <v>205</v>
       </c>
-      <c r="G108" s="92"/>
-      <c r="H108" s="93"/>
+      <c r="G108" s="79"/>
+      <c r="H108" s="80"/>
       <c r="I108" s="9"/>
       <c r="J108" s="2"/>
       <c r="K108" s="3"/>
@@ -6795,18 +6801,18 @@
       <c r="Z108" s="3"/>
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="78"/>
-      <c r="B109" s="91" t="s">
+      <c r="A109" s="84"/>
+      <c r="B109" s="78" t="s">
         <v>480</v>
       </c>
-      <c r="C109" s="92"/>
-      <c r="D109" s="93"/>
-      <c r="E109" s="99"/>
-      <c r="F109" s="91" t="s">
+      <c r="C109" s="79"/>
+      <c r="D109" s="80"/>
+      <c r="E109" s="88"/>
+      <c r="F109" s="78" t="s">
         <v>206</v>
       </c>
-      <c r="G109" s="92"/>
-      <c r="H109" s="93"/>
+      <c r="G109" s="79"/>
+      <c r="H109" s="80"/>
       <c r="I109" s="9"/>
       <c r="J109" s="2"/>
       <c r="K109" s="3"/>
@@ -6855,7 +6861,7 @@
       <c r="Z110" s="3"/>
     </row>
     <row r="111" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="76" t="s">
+      <c r="A111" s="126" t="s">
         <v>207</v>
       </c>
       <c r="B111" s="51"/>
@@ -6865,7 +6871,7 @@
       <c r="D111" s="65" t="s">
         <v>552</v>
       </c>
-      <c r="E111" s="79" t="s">
+      <c r="E111" s="127" t="s">
         <v>13</v>
       </c>
       <c r="F111" s="47" t="s">
@@ -6899,7 +6905,7 @@
       <c r="Z111" s="3"/>
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="77"/>
+      <c r="A112" s="82"/>
       <c r="B112" s="48"/>
       <c r="C112" s="47" t="s">
         <v>175</v>
@@ -6907,7 +6913,7 @@
       <c r="D112" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="E112" s="80"/>
+      <c r="E112" s="128"/>
       <c r="F112" s="47" t="s">
         <v>17</v>
       </c>
@@ -6937,7 +6943,7 @@
       <c r="Z112" s="3"/>
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="77"/>
+      <c r="A113" s="82"/>
       <c r="B113" s="48"/>
       <c r="C113" s="47" t="s">
         <v>83</v>
@@ -6945,7 +6951,7 @@
       <c r="D113" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="E113" s="80"/>
+      <c r="E113" s="128"/>
       <c r="F113" s="47" t="s">
         <v>22</v>
       </c>
@@ -6974,12 +6980,12 @@
       <c r="Z113" s="3"/>
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="77"/>
+      <c r="A114" s="82"/>
       <c r="B114" s="48"/>
       <c r="D114" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="E114" s="80"/>
+      <c r="E114" s="128"/>
       <c r="F114" s="47" t="s">
         <v>42</v>
       </c>
@@ -7011,7 +7017,7 @@
       <c r="Z114" s="3"/>
     </row>
     <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="77"/>
+      <c r="A115" s="82"/>
       <c r="B115" s="50"/>
       <c r="C115" s="47" t="s">
         <v>92</v>
@@ -7019,7 +7025,7 @@
       <c r="D115" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="E115" s="80"/>
+      <c r="E115" s="128"/>
       <c r="F115" s="47" t="s">
         <v>27</v>
       </c>
@@ -7051,7 +7057,7 @@
       <c r="Z115" s="3"/>
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="77"/>
+      <c r="A116" s="82"/>
       <c r="B116" s="74" t="s">
         <v>608</v>
       </c>
@@ -7061,7 +7067,7 @@
       <c r="D116" s="65" t="s">
         <v>544</v>
       </c>
-      <c r="E116" s="80"/>
+      <c r="E116" s="128"/>
       <c r="F116" s="47" t="s">
         <v>32</v>
       </c>
@@ -7093,7 +7099,7 @@
       <c r="Z116" s="3"/>
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="77"/>
+      <c r="A117" s="82"/>
       <c r="B117" s="47" t="s">
         <v>594</v>
       </c>
@@ -7103,7 +7109,7 @@
       <c r="D117" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="E117" s="80"/>
+      <c r="E117" s="128"/>
       <c r="F117" s="65" t="s">
         <v>215</v>
       </c>
@@ -7135,7 +7141,7 @@
       <c r="Z117" s="3"/>
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="77"/>
+      <c r="A118" s="82"/>
       <c r="B118" s="47" t="s">
         <v>217</v>
       </c>
@@ -7145,7 +7151,7 @@
       <c r="D118" s="65" t="s">
         <v>543</v>
       </c>
-      <c r="E118" s="80"/>
+      <c r="E118" s="128"/>
       <c r="F118" s="47" t="s">
         <v>36</v>
       </c>
@@ -7175,7 +7181,7 @@
       <c r="Z118" s="3"/>
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="77"/>
+      <c r="A119" s="82"/>
       <c r="B119" s="47" t="s">
         <v>458</v>
       </c>
@@ -7185,11 +7191,13 @@
       <c r="D119" s="63" t="s">
         <v>521</v>
       </c>
-      <c r="E119" s="80"/>
+      <c r="E119" s="128"/>
       <c r="F119" s="47" t="s">
         <v>219</v>
       </c>
-      <c r="G119" s="48"/>
+      <c r="G119" s="133" t="s">
+        <v>182</v>
+      </c>
       <c r="H119" s="51"/>
       <c r="I119" s="48"/>
       <c r="J119" s="2"/>
@@ -7211,7 +7219,7 @@
       <c r="Z119" s="3"/>
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="77"/>
+      <c r="A120" s="82"/>
       <c r="B120" s="47" t="s">
         <v>220</v>
       </c>
@@ -7221,7 +7229,7 @@
       <c r="D120" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="E120" s="80"/>
+      <c r="E120" s="128"/>
       <c r="F120" s="65" t="s">
         <v>578</v>
       </c>
@@ -7249,7 +7257,7 @@
       <c r="Z120" s="3"/>
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="77"/>
+      <c r="A121" s="82"/>
       <c r="B121" s="47" t="s">
         <v>223</v>
       </c>
@@ -7259,7 +7267,7 @@
       <c r="D121" s="47" t="s">
         <v>225</v>
       </c>
-      <c r="E121" s="80"/>
+      <c r="E121" s="128"/>
       <c r="F121" s="50" t="s">
         <v>226</v>
       </c>
@@ -7285,21 +7293,21 @@
       <c r="Z121" s="3"/>
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="77"/>
+      <c r="A122" s="82"/>
       <c r="B122" s="50" t="s">
         <v>441</v>
       </c>
       <c r="C122" s="48"/>
       <c r="D122" s="51"/>
-      <c r="E122" s="80"/>
-      <c r="F122" s="84" t="s">
+      <c r="E122" s="128"/>
+      <c r="F122" s="94" t="s">
         <v>477</v>
       </c>
-      <c r="G122" s="85"/>
-      <c r="H122" s="84" t="s">
+      <c r="G122" s="77"/>
+      <c r="H122" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="I122" s="85"/>
+      <c r="I122" s="77"/>
       <c r="J122" s="2"/>
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
@@ -7319,21 +7327,21 @@
       <c r="Z122" s="3"/>
     </row>
     <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="77"/>
+      <c r="A123" s="82"/>
       <c r="B123" s="49"/>
       <c r="C123" s="48"/>
       <c r="D123" s="50" t="s">
         <v>228</v>
       </c>
-      <c r="E123" s="80"/>
-      <c r="F123" s="84" t="s">
+      <c r="E123" s="128"/>
+      <c r="F123" s="94" t="s">
         <v>459</v>
       </c>
-      <c r="G123" s="85"/>
-      <c r="H123" s="84" t="s">
+      <c r="G123" s="77"/>
+      <c r="H123" s="94" t="s">
         <v>229</v>
       </c>
-      <c r="I123" s="85"/>
+      <c r="I123" s="77"/>
       <c r="J123" s="2"/>
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
@@ -7353,21 +7361,21 @@
       <c r="Z123" s="3"/>
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="77"/>
+      <c r="A124" s="82"/>
       <c r="B124" s="50"/>
-      <c r="C124" s="82" t="s">
+      <c r="C124" s="91" t="s">
         <v>576</v>
       </c>
-      <c r="D124" s="83"/>
-      <c r="E124" s="80"/>
-      <c r="F124" s="82" t="s">
+      <c r="D124" s="92"/>
+      <c r="E124" s="128"/>
+      <c r="F124" s="91" t="s">
         <v>580</v>
       </c>
-      <c r="G124" s="83"/>
-      <c r="H124" s="82" t="s">
+      <c r="G124" s="92"/>
+      <c r="H124" s="91" t="s">
         <v>582</v>
       </c>
-      <c r="I124" s="83"/>
+      <c r="I124" s="92"/>
       <c r="J124" s="2"/>
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
@@ -7387,21 +7395,21 @@
       <c r="Z124" s="3"/>
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="77"/>
+      <c r="A125" s="82"/>
       <c r="B125" s="47"/>
-      <c r="C125" s="82" t="s">
+      <c r="C125" s="91" t="s">
         <v>577</v>
       </c>
-      <c r="D125" s="82"/>
-      <c r="E125" s="80"/>
-      <c r="F125" s="82" t="s">
+      <c r="D125" s="91"/>
+      <c r="E125" s="128"/>
+      <c r="F125" s="91" t="s">
         <v>581</v>
       </c>
-      <c r="G125" s="83"/>
-      <c r="H125" s="82" t="s">
+      <c r="G125" s="92"/>
+      <c r="H125" s="91" t="s">
         <v>583</v>
       </c>
-      <c r="I125" s="83"/>
+      <c r="I125" s="92"/>
       <c r="J125" s="2"/>
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
@@ -7421,21 +7429,21 @@
       <c r="Z125" s="3"/>
     </row>
     <row r="126" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="77"/>
+      <c r="A126" s="82"/>
       <c r="B126" s="50"/>
-      <c r="C126" s="84" t="s">
+      <c r="C126" s="94" t="s">
         <v>493</v>
       </c>
-      <c r="D126" s="85"/>
-      <c r="E126" s="80"/>
-      <c r="F126" s="84" t="s">
+      <c r="D126" s="77"/>
+      <c r="E126" s="128"/>
+      <c r="F126" s="94" t="s">
         <v>230</v>
       </c>
-      <c r="G126" s="85"/>
-      <c r="H126" s="84" t="s">
+      <c r="G126" s="77"/>
+      <c r="H126" s="94" t="s">
         <v>483</v>
       </c>
-      <c r="I126" s="85"/>
+      <c r="I126" s="77"/>
       <c r="J126" s="2"/>
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
@@ -7455,21 +7463,21 @@
       <c r="Z126" s="3"/>
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="77"/>
+      <c r="A127" s="82"/>
       <c r="B127" s="48"/>
-      <c r="C127" s="84" t="s">
+      <c r="C127" s="94" t="s">
         <v>231</v>
       </c>
-      <c r="D127" s="85"/>
-      <c r="E127" s="80"/>
-      <c r="F127" s="84" t="s">
+      <c r="D127" s="77"/>
+      <c r="E127" s="128"/>
+      <c r="F127" s="94" t="s">
         <v>232</v>
       </c>
-      <c r="G127" s="85"/>
-      <c r="H127" s="84" t="s">
+      <c r="G127" s="77"/>
+      <c r="H127" s="94" t="s">
         <v>233</v>
       </c>
-      <c r="I127" s="85"/>
+      <c r="I127" s="77"/>
       <c r="J127" s="2"/>
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
@@ -7489,21 +7497,21 @@
       <c r="Z127" s="3"/>
     </row>
     <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="77"/>
+      <c r="A128" s="82"/>
       <c r="B128" s="48"/>
-      <c r="C128" s="84" t="s">
+      <c r="C128" s="94" t="s">
         <v>476</v>
       </c>
-      <c r="D128" s="85"/>
-      <c r="E128" s="80"/>
-      <c r="F128" s="94" t="s">
+      <c r="D128" s="77"/>
+      <c r="E128" s="128"/>
+      <c r="F128" s="98" t="s">
         <v>508</v>
       </c>
-      <c r="G128" s="118"/>
-      <c r="H128" s="94" t="s">
+      <c r="G128" s="107"/>
+      <c r="H128" s="98" t="s">
         <v>433</v>
       </c>
-      <c r="I128" s="85"/>
+      <c r="I128" s="77"/>
       <c r="J128" s="2"/>
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
@@ -7523,21 +7531,21 @@
       <c r="Z128" s="3"/>
     </row>
     <row r="129" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="77"/>
-      <c r="B129" s="84" t="s">
+      <c r="A129" s="82"/>
+      <c r="B129" s="94" t="s">
         <v>234</v>
       </c>
-      <c r="C129" s="85"/>
+      <c r="C129" s="77"/>
       <c r="D129" s="48"/>
-      <c r="E129" s="80"/>
-      <c r="F129" s="117" t="s">
+      <c r="E129" s="128"/>
+      <c r="F129" s="101" t="s">
         <v>235</v>
       </c>
-      <c r="G129" s="85"/>
-      <c r="H129" s="94" t="s">
+      <c r="G129" s="77"/>
+      <c r="H129" s="98" t="s">
         <v>506</v>
       </c>
-      <c r="I129" s="85"/>
+      <c r="I129" s="77"/>
       <c r="J129" s="2"/>
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
@@ -7557,15 +7565,15 @@
       <c r="Z129" s="3"/>
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="77"/>
+      <c r="A130" s="82"/>
       <c r="B130" s="47"/>
       <c r="C130" s="48"/>
       <c r="D130" s="48"/>
-      <c r="E130" s="80"/>
-      <c r="F130" s="84" t="s">
+      <c r="E130" s="128"/>
+      <c r="F130" s="94" t="s">
         <v>236</v>
       </c>
-      <c r="G130" s="85"/>
+      <c r="G130" s="77"/>
       <c r="H130" s="53"/>
       <c r="I130" s="53"/>
       <c r="J130" s="2"/>
@@ -7587,13 +7595,13 @@
       <c r="Z130" s="3"/>
     </row>
     <row r="131" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="77"/>
+      <c r="A131" s="82"/>
       <c r="B131" s="47"/>
       <c r="C131" s="48"/>
       <c r="D131" s="48"/>
-      <c r="E131" s="80"/>
-      <c r="F131" s="94"/>
-      <c r="G131" s="85"/>
+      <c r="E131" s="128"/>
+      <c r="F131" s="98"/>
+      <c r="G131" s="77"/>
       <c r="H131" s="47"/>
       <c r="I131" s="47"/>
       <c r="J131" s="2"/>
@@ -7615,18 +7623,18 @@
       <c r="Z131" s="3"/>
     </row>
     <row r="132" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="77"/>
-      <c r="B132" s="84" t="s">
+      <c r="A132" s="82"/>
+      <c r="B132" s="94" t="s">
         <v>463</v>
       </c>
-      <c r="C132" s="86"/>
-      <c r="D132" s="85"/>
-      <c r="E132" s="80"/>
-      <c r="F132" s="84" t="s">
+      <c r="C132" s="93"/>
+      <c r="D132" s="77"/>
+      <c r="E132" s="128"/>
+      <c r="F132" s="94" t="s">
         <v>237</v>
       </c>
-      <c r="G132" s="86"/>
-      <c r="H132" s="85"/>
+      <c r="G132" s="93"/>
+      <c r="H132" s="77"/>
       <c r="I132" s="50"/>
       <c r="J132" s="2"/>
       <c r="K132" s="3"/>
@@ -7647,18 +7655,18 @@
       <c r="Z132" s="3"/>
     </row>
     <row r="133" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="77"/>
-      <c r="B133" s="84" t="s">
+      <c r="A133" s="82"/>
+      <c r="B133" s="94" t="s">
         <v>238</v>
       </c>
-      <c r="C133" s="86"/>
-      <c r="D133" s="85"/>
-      <c r="E133" s="80"/>
-      <c r="F133" s="84" t="s">
+      <c r="C133" s="93"/>
+      <c r="D133" s="77"/>
+      <c r="E133" s="128"/>
+      <c r="F133" s="94" t="s">
         <v>239</v>
       </c>
-      <c r="G133" s="86"/>
-      <c r="H133" s="85"/>
+      <c r="G133" s="93"/>
+      <c r="H133" s="77"/>
       <c r="I133" s="50"/>
       <c r="J133" s="2"/>
       <c r="K133" s="3"/>
@@ -7679,18 +7687,18 @@
       <c r="Z133" s="3"/>
     </row>
     <row r="134" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="77"/>
-      <c r="B134" s="84" t="s">
+      <c r="A134" s="82"/>
+      <c r="B134" s="94" t="s">
         <v>240</v>
       </c>
-      <c r="C134" s="86"/>
-      <c r="D134" s="85"/>
-      <c r="E134" s="80"/>
-      <c r="F134" s="84" t="s">
+      <c r="C134" s="93"/>
+      <c r="D134" s="77"/>
+      <c r="E134" s="128"/>
+      <c r="F134" s="94" t="s">
         <v>471</v>
       </c>
-      <c r="G134" s="86"/>
-      <c r="H134" s="85"/>
+      <c r="G134" s="93"/>
+      <c r="H134" s="77"/>
       <c r="I134" s="50"/>
       <c r="J134" s="2"/>
       <c r="K134" s="3"/>
@@ -7711,16 +7719,16 @@
       <c r="Z134" s="3"/>
     </row>
     <row r="135" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="78"/>
-      <c r="B135" s="84"/>
-      <c r="C135" s="86"/>
-      <c r="D135" s="85"/>
-      <c r="E135" s="81"/>
-      <c r="F135" s="84" t="s">
+      <c r="A135" s="84"/>
+      <c r="B135" s="94"/>
+      <c r="C135" s="93"/>
+      <c r="D135" s="77"/>
+      <c r="E135" s="129"/>
+      <c r="F135" s="94" t="s">
         <v>472</v>
       </c>
-      <c r="G135" s="86"/>
-      <c r="H135" s="85"/>
+      <c r="G135" s="93"/>
+      <c r="H135" s="77"/>
       <c r="I135" s="50"/>
       <c r="J135" s="2"/>
       <c r="K135" s="3"/>
@@ -7769,7 +7777,7 @@
       <c r="Z136" s="3"/>
     </row>
     <row r="137" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="87" t="s">
+      <c r="A137" s="130" t="s">
         <v>241</v>
       </c>
       <c r="B137" s="8" t="s">
@@ -7784,9 +7792,9 @@
       <c r="E137" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F137" s="91"/>
-      <c r="G137" s="92"/>
-      <c r="H137" s="93"/>
+      <c r="F137" s="78"/>
+      <c r="G137" s="79"/>
+      <c r="H137" s="80"/>
       <c r="I137" s="8"/>
       <c r="J137" s="2"/>
       <c r="K137" s="3"/>
@@ -7807,7 +7815,7 @@
       <c r="Z137" s="3"/>
     </row>
     <row r="138" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="77"/>
+      <c r="A138" s="82"/>
       <c r="B138" s="40" t="s">
         <v>243</v>
       </c>
@@ -7843,7 +7851,7 @@
       <c r="Z138" s="3"/>
     </row>
     <row r="139" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="77"/>
+      <c r="A139" s="82"/>
       <c r="B139" s="41" t="s">
         <v>246</v>
       </c>
@@ -7877,7 +7885,7 @@
       <c r="Z139" s="3"/>
     </row>
     <row r="140" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="77"/>
+      <c r="A140" s="82"/>
       <c r="B140" s="41" t="s">
         <v>247</v>
       </c>
@@ -7910,7 +7918,7 @@
       <c r="Z140" s="3"/>
     </row>
     <row r="141" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="77"/>
+      <c r="A141" s="82"/>
       <c r="B141" s="40" t="s">
         <v>248</v>
       </c>
@@ -7944,7 +7952,7 @@
       <c r="Z141" s="3"/>
     </row>
     <row r="142" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="77"/>
+      <c r="A142" s="82"/>
       <c r="B142" s="40" t="s">
         <v>249</v>
       </c>
@@ -7978,7 +7986,7 @@
       <c r="Z142" s="3"/>
     </row>
     <row r="143" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="77"/>
+      <c r="A143" s="82"/>
       <c r="B143" s="46"/>
       <c r="C143" s="40" t="s">
         <v>251</v>
@@ -8010,7 +8018,7 @@
       <c r="Z143" s="3"/>
     </row>
     <row r="144" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="77"/>
+      <c r="A144" s="82"/>
       <c r="B144" s="41" t="s">
         <v>252</v>
       </c>
@@ -8044,7 +8052,7 @@
       <c r="Z144" s="3"/>
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="77"/>
+      <c r="A145" s="82"/>
       <c r="B145" s="41" t="s">
         <v>444</v>
       </c>
@@ -8078,7 +8086,7 @@
       <c r="Z145" s="3"/>
     </row>
     <row r="146" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="77"/>
+      <c r="A146" s="82"/>
       <c r="B146" s="38"/>
       <c r="C146" s="41" t="s">
         <v>257</v>
@@ -8108,7 +8116,7 @@
       <c r="Z146" s="3"/>
     </row>
     <row r="147" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="77"/>
+      <c r="A147" s="82"/>
       <c r="B147" s="38"/>
       <c r="C147" s="63" t="s">
         <v>258</v>
@@ -8138,7 +8146,7 @@
       <c r="Z147" s="3"/>
     </row>
     <row r="148" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="77"/>
+      <c r="A148" s="82"/>
       <c r="B148" s="38"/>
       <c r="C148" s="41"/>
       <c r="D148" s="42"/>
@@ -8166,13 +8174,13 @@
       <c r="Z148" s="3"/>
     </row>
     <row r="149" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="77"/>
+      <c r="A149" s="82"/>
       <c r="B149" s="38"/>
       <c r="C149" s="46"/>
-      <c r="D149" s="88" t="s">
+      <c r="D149" s="89" t="s">
         <v>259</v>
       </c>
-      <c r="E149" s="85"/>
+      <c r="E149" s="77"/>
       <c r="F149" s="10"/>
       <c r="G149" s="8"/>
       <c r="H149" s="8"/>
@@ -8196,15 +8204,15 @@
       <c r="Z149" s="3"/>
     </row>
     <row r="150" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="77"/>
-      <c r="B150" s="89" t="s">
+      <c r="A150" s="82"/>
+      <c r="B150" s="131" t="s">
         <v>584</v>
       </c>
-      <c r="C150" s="90"/>
-      <c r="D150" s="88" t="s">
+      <c r="C150" s="132"/>
+      <c r="D150" s="89" t="s">
         <v>492</v>
       </c>
-      <c r="E150" s="85"/>
+      <c r="E150" s="77"/>
       <c r="F150" s="8"/>
       <c r="G150" s="8"/>
       <c r="H150" s="8"/>
@@ -8228,15 +8236,15 @@
       <c r="Z150" s="3"/>
     </row>
     <row r="151" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="77"/>
-      <c r="B151" s="82" t="s">
+      <c r="A151" s="82"/>
+      <c r="B151" s="91" t="s">
         <v>585</v>
       </c>
-      <c r="C151" s="83"/>
-      <c r="D151" s="88" t="s">
+      <c r="C151" s="92"/>
+      <c r="D151" s="89" t="s">
         <v>598</v>
       </c>
-      <c r="E151" s="85"/>
+      <c r="E151" s="77"/>
       <c r="F151" s="8"/>
       <c r="G151" s="8"/>
       <c r="H151" s="8"/>
@@ -8260,15 +8268,15 @@
       <c r="Z151" s="3"/>
     </row>
     <row r="152" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="77"/>
-      <c r="B152" s="88" t="s">
+      <c r="A152" s="82"/>
+      <c r="B152" s="89" t="s">
         <v>260</v>
       </c>
-      <c r="C152" s="85"/>
-      <c r="D152" s="103" t="s">
+      <c r="C152" s="77"/>
+      <c r="D152" s="97" t="s">
         <v>261</v>
       </c>
-      <c r="E152" s="85"/>
+      <c r="E152" s="77"/>
       <c r="F152" s="8"/>
       <c r="G152" s="8"/>
       <c r="H152" s="8"/>
@@ -8292,15 +8300,15 @@
       <c r="Z152" s="3"/>
     </row>
     <row r="153" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="77"/>
-      <c r="B153" s="88" t="s">
+      <c r="A153" s="82"/>
+      <c r="B153" s="89" t="s">
         <v>262</v>
       </c>
-      <c r="C153" s="85"/>
-      <c r="D153" s="94" t="s">
+      <c r="C153" s="77"/>
+      <c r="D153" s="98" t="s">
         <v>517</v>
       </c>
-      <c r="E153" s="85"/>
+      <c r="E153" s="77"/>
       <c r="F153" s="8"/>
       <c r="G153" s="8"/>
       <c r="H153" s="8"/>
@@ -8324,15 +8332,15 @@
       <c r="Z153" s="3"/>
     </row>
     <row r="154" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="77"/>
-      <c r="B154" s="103" t="s">
+      <c r="A154" s="82"/>
+      <c r="B154" s="97" t="s">
         <v>263</v>
       </c>
-      <c r="C154" s="85"/>
-      <c r="D154" s="88" t="s">
+      <c r="C154" s="77"/>
+      <c r="D154" s="89" t="s">
         <v>264</v>
       </c>
-      <c r="E154" s="85"/>
+      <c r="E154" s="77"/>
       <c r="F154" s="8"/>
       <c r="G154" s="8"/>
       <c r="H154" s="8"/>
@@ -8356,15 +8364,15 @@
       <c r="Z154" s="3"/>
     </row>
     <row r="155" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="77"/>
-      <c r="B155" s="103" t="s">
+      <c r="A155" s="82"/>
+      <c r="B155" s="97" t="s">
         <v>427</v>
       </c>
-      <c r="C155" s="85"/>
-      <c r="D155" s="107" t="s">
+      <c r="C155" s="77"/>
+      <c r="D155" s="116" t="s">
         <v>604</v>
       </c>
-      <c r="E155" s="108"/>
+      <c r="E155" s="117"/>
       <c r="F155" s="8"/>
       <c r="G155" s="8"/>
       <c r="H155" s="8"/>
@@ -8388,11 +8396,11 @@
       <c r="Z155" s="3"/>
     </row>
     <row r="156" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="77"/>
-      <c r="B156" s="88" t="s">
+      <c r="A156" s="82"/>
+      <c r="B156" s="89" t="s">
         <v>265</v>
       </c>
-      <c r="C156" s="85"/>
+      <c r="C156" s="77"/>
       <c r="D156" s="40"/>
       <c r="E156" s="41"/>
       <c r="F156" s="8"/>
@@ -8418,11 +8426,11 @@
       <c r="Z156" s="3"/>
     </row>
     <row r="157" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="77"/>
-      <c r="B157" s="88" t="s">
+      <c r="A157" s="82"/>
+      <c r="B157" s="89" t="s">
         <v>266</v>
       </c>
-      <c r="C157" s="85"/>
+      <c r="C157" s="77"/>
       <c r="D157" s="40"/>
       <c r="E157" s="41"/>
       <c r="F157" s="8"/>
@@ -8448,12 +8456,12 @@
       <c r="Z157" s="3"/>
     </row>
     <row r="158" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="77"/>
-      <c r="B158" s="88" t="s">
+      <c r="A158" s="82"/>
+      <c r="B158" s="89" t="s">
         <v>464</v>
       </c>
-      <c r="C158" s="86"/>
-      <c r="D158" s="85"/>
+      <c r="C158" s="93"/>
+      <c r="D158" s="77"/>
       <c r="E158" s="41"/>
       <c r="F158" s="8"/>
       <c r="G158" s="8"/>
@@ -8478,12 +8486,12 @@
       <c r="Z158" s="3"/>
     </row>
     <row r="159" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="77"/>
-      <c r="B159" s="88" t="s">
+      <c r="A159" s="82"/>
+      <c r="B159" s="89" t="s">
         <v>267</v>
       </c>
-      <c r="C159" s="86"/>
-      <c r="D159" s="85"/>
+      <c r="C159" s="93"/>
+      <c r="D159" s="77"/>
       <c r="E159" s="41"/>
       <c r="F159" s="8"/>
       <c r="G159" s="8"/>
@@ -8508,12 +8516,12 @@
       <c r="Z159" s="3"/>
     </row>
     <row r="160" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="77"/>
-      <c r="B160" s="88" t="s">
+      <c r="A160" s="82"/>
+      <c r="B160" s="89" t="s">
         <v>268</v>
       </c>
-      <c r="C160" s="86"/>
-      <c r="D160" s="85"/>
+      <c r="C160" s="93"/>
+      <c r="D160" s="77"/>
       <c r="E160" s="41"/>
       <c r="F160" s="8"/>
       <c r="G160" s="8"/>
@@ -8538,12 +8546,12 @@
       <c r="Z160" s="3"/>
     </row>
     <row r="161" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="78"/>
-      <c r="B161" s="88" t="s">
+      <c r="A161" s="84"/>
+      <c r="B161" s="89" t="s">
         <v>465</v>
       </c>
-      <c r="C161" s="86"/>
-      <c r="D161" s="85"/>
+      <c r="C161" s="93"/>
+      <c r="D161" s="77"/>
       <c r="E161" s="41"/>
       <c r="F161" s="8"/>
       <c r="G161" s="8"/>
@@ -8596,17 +8604,17 @@
       <c r="Z162" s="3"/>
     </row>
     <row r="163" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="109" t="s">
+      <c r="A163" s="113" t="s">
         <v>269</v>
       </c>
-      <c r="B163" s="110"/>
-      <c r="C163" s="110"/>
-      <c r="D163" s="110"/>
-      <c r="E163" s="110"/>
-      <c r="F163" s="110"/>
-      <c r="G163" s="110"/>
-      <c r="H163" s="110"/>
-      <c r="I163" s="111"/>
+      <c r="B163" s="114"/>
+      <c r="C163" s="114"/>
+      <c r="D163" s="114"/>
+      <c r="E163" s="114"/>
+      <c r="F163" s="114"/>
+      <c r="G163" s="114"/>
+      <c r="H163" s="114"/>
+      <c r="I163" s="115"/>
       <c r="J163" s="2"/>
       <c r="K163" s="3"/>
       <c r="L163" s="3"/>
@@ -8654,17 +8662,17 @@
       <c r="Z164" s="3"/>
     </row>
     <row r="165" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="112" t="s">
+      <c r="A165" s="109" t="s">
         <v>270</v>
       </c>
-      <c r="B165" s="92"/>
-      <c r="C165" s="92"/>
-      <c r="D165" s="92"/>
-      <c r="E165" s="92"/>
-      <c r="F165" s="92"/>
-      <c r="G165" s="92"/>
-      <c r="H165" s="92"/>
-      <c r="I165" s="93"/>
+      <c r="B165" s="79"/>
+      <c r="C165" s="79"/>
+      <c r="D165" s="79"/>
+      <c r="E165" s="79"/>
+      <c r="F165" s="79"/>
+      <c r="G165" s="79"/>
+      <c r="H165" s="79"/>
+      <c r="I165" s="80"/>
       <c r="J165" s="2"/>
       <c r="K165" s="3"/>
       <c r="L165" s="3"/>
@@ -8685,16 +8693,16 @@
     </row>
     <row r="166" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="24"/>
-      <c r="B166" s="91" t="s">
+      <c r="B166" s="78" t="s">
         <v>271</v>
       </c>
-      <c r="C166" s="92"/>
-      <c r="D166" s="92"/>
-      <c r="E166" s="92"/>
-      <c r="F166" s="92"/>
-      <c r="G166" s="92"/>
-      <c r="H166" s="92"/>
-      <c r="I166" s="93"/>
+      <c r="C166" s="79"/>
+      <c r="D166" s="79"/>
+      <c r="E166" s="79"/>
+      <c r="F166" s="79"/>
+      <c r="G166" s="79"/>
+      <c r="H166" s="79"/>
+      <c r="I166" s="80"/>
       <c r="J166" s="2"/>
       <c r="K166" s="3"/>
       <c r="L166" s="3"/>
@@ -8715,16 +8723,16 @@
     </row>
     <row r="167" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="24"/>
-      <c r="B167" s="91" t="s">
+      <c r="B167" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="C167" s="92"/>
-      <c r="D167" s="92"/>
-      <c r="E167" s="92"/>
-      <c r="F167" s="92"/>
-      <c r="G167" s="92"/>
-      <c r="H167" s="92"/>
-      <c r="I167" s="93"/>
+      <c r="C167" s="79"/>
+      <c r="D167" s="79"/>
+      <c r="E167" s="79"/>
+      <c r="F167" s="79"/>
+      <c r="G167" s="79"/>
+      <c r="H167" s="79"/>
+      <c r="I167" s="80"/>
       <c r="J167" s="2"/>
       <c r="K167" s="3"/>
       <c r="L167" s="3"/>
@@ -8745,16 +8753,16 @@
     </row>
     <row r="168" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="24"/>
-      <c r="B168" s="91" t="s">
+      <c r="B168" s="78" t="s">
         <v>273</v>
       </c>
-      <c r="C168" s="92"/>
-      <c r="D168" s="92"/>
-      <c r="E168" s="92"/>
-      <c r="F168" s="92"/>
-      <c r="G168" s="92"/>
-      <c r="H168" s="92"/>
-      <c r="I168" s="93"/>
+      <c r="C168" s="79"/>
+      <c r="D168" s="79"/>
+      <c r="E168" s="79"/>
+      <c r="F168" s="79"/>
+      <c r="G168" s="79"/>
+      <c r="H168" s="79"/>
+      <c r="I168" s="80"/>
       <c r="J168" s="2"/>
       <c r="K168" s="3"/>
       <c r="L168" s="3"/>
@@ -8775,16 +8783,16 @@
     </row>
     <row r="169" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="24"/>
-      <c r="B169" s="91" t="s">
+      <c r="B169" s="78" t="s">
         <v>274</v>
       </c>
-      <c r="C169" s="92"/>
-      <c r="D169" s="92"/>
-      <c r="E169" s="92"/>
-      <c r="F169" s="92"/>
-      <c r="G169" s="92"/>
-      <c r="H169" s="92"/>
-      <c r="I169" s="93"/>
+      <c r="C169" s="79"/>
+      <c r="D169" s="79"/>
+      <c r="E169" s="79"/>
+      <c r="F169" s="79"/>
+      <c r="G169" s="79"/>
+      <c r="H169" s="79"/>
+      <c r="I169" s="80"/>
       <c r="J169" s="2"/>
       <c r="K169" s="3"/>
       <c r="L169" s="3"/>
@@ -8805,16 +8813,16 @@
     </row>
     <row r="170" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="24"/>
-      <c r="B170" s="91" t="s">
+      <c r="B170" s="78" t="s">
         <v>275</v>
       </c>
-      <c r="C170" s="92"/>
-      <c r="D170" s="92"/>
-      <c r="E170" s="92"/>
-      <c r="F170" s="92"/>
-      <c r="G170" s="92"/>
-      <c r="H170" s="92"/>
-      <c r="I170" s="93"/>
+      <c r="C170" s="79"/>
+      <c r="D170" s="79"/>
+      <c r="E170" s="79"/>
+      <c r="F170" s="79"/>
+      <c r="G170" s="79"/>
+      <c r="H170" s="79"/>
+      <c r="I170" s="80"/>
       <c r="J170" s="2"/>
       <c r="K170" s="3"/>
       <c r="L170" s="3"/>
@@ -8835,16 +8843,16 @@
     </row>
     <row r="171" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="24"/>
-      <c r="B171" s="114" t="s">
+      <c r="B171" s="110" t="s">
         <v>276</v>
       </c>
-      <c r="C171" s="92"/>
-      <c r="D171" s="92"/>
-      <c r="E171" s="92"/>
-      <c r="F171" s="92"/>
-      <c r="G171" s="92"/>
-      <c r="H171" s="92"/>
-      <c r="I171" s="93"/>
+      <c r="C171" s="79"/>
+      <c r="D171" s="79"/>
+      <c r="E171" s="79"/>
+      <c r="F171" s="79"/>
+      <c r="G171" s="79"/>
+      <c r="H171" s="79"/>
+      <c r="I171" s="80"/>
       <c r="J171" s="2"/>
       <c r="K171" s="3"/>
       <c r="L171" s="3"/>
@@ -8864,17 +8872,17 @@
       <c r="Z171" s="3"/>
     </row>
     <row r="172" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="112" t="s">
+      <c r="A172" s="109" t="s">
         <v>277</v>
       </c>
-      <c r="B172" s="92"/>
-      <c r="C172" s="92"/>
-      <c r="D172" s="92"/>
-      <c r="E172" s="92"/>
-      <c r="F172" s="92"/>
-      <c r="G172" s="92"/>
-      <c r="H172" s="92"/>
-      <c r="I172" s="93"/>
+      <c r="B172" s="79"/>
+      <c r="C172" s="79"/>
+      <c r="D172" s="79"/>
+      <c r="E172" s="79"/>
+      <c r="F172" s="79"/>
+      <c r="G172" s="79"/>
+      <c r="H172" s="79"/>
+      <c r="I172" s="80"/>
       <c r="J172" s="2"/>
       <c r="K172" s="3"/>
       <c r="L172" s="3"/>
@@ -8894,21 +8902,21 @@
       <c r="Z172" s="3"/>
     </row>
     <row r="173" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="115"/>
+      <c r="A173" s="111"/>
       <c r="B173" s="24" t="s">
         <v>278</v>
       </c>
       <c r="C173" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="D173" s="113" t="s">
+      <c r="D173" s="108" t="s">
         <v>279</v>
       </c>
-      <c r="E173" s="92"/>
-      <c r="F173" s="92"/>
-      <c r="G173" s="92"/>
-      <c r="H173" s="92"/>
-      <c r="I173" s="93"/>
+      <c r="E173" s="79"/>
+      <c r="F173" s="79"/>
+      <c r="G173" s="79"/>
+      <c r="H173" s="79"/>
+      <c r="I173" s="80"/>
       <c r="J173" s="2"/>
       <c r="K173" s="3"/>
       <c r="L173" s="3"/>
@@ -8928,19 +8936,19 @@
       <c r="Z173" s="3"/>
     </row>
     <row r="174" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="98"/>
+      <c r="A174" s="86"/>
       <c r="B174" s="24"/>
       <c r="C174" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="D174" s="116" t="s">
+      <c r="D174" s="112" t="s">
         <v>281</v>
       </c>
-      <c r="E174" s="92"/>
-      <c r="F174" s="92"/>
-      <c r="G174" s="92"/>
-      <c r="H174" s="92"/>
-      <c r="I174" s="93"/>
+      <c r="E174" s="79"/>
+      <c r="F174" s="79"/>
+      <c r="G174" s="79"/>
+      <c r="H174" s="79"/>
+      <c r="I174" s="80"/>
       <c r="J174" s="2"/>
       <c r="K174" s="3"/>
       <c r="L174" s="3"/>
@@ -8960,19 +8968,19 @@
       <c r="Z174" s="3"/>
     </row>
     <row r="175" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="99"/>
+      <c r="A175" s="88"/>
       <c r="B175" s="24"/>
       <c r="C175" s="63" t="s">
         <v>282</v>
       </c>
-      <c r="D175" s="113" t="s">
+      <c r="D175" s="108" t="s">
         <v>283</v>
       </c>
-      <c r="E175" s="92"/>
-      <c r="F175" s="92"/>
-      <c r="G175" s="92"/>
-      <c r="H175" s="92"/>
-      <c r="I175" s="93"/>
+      <c r="E175" s="79"/>
+      <c r="F175" s="79"/>
+      <c r="G175" s="79"/>
+      <c r="H175" s="79"/>
+      <c r="I175" s="80"/>
       <c r="J175" s="2"/>
       <c r="K175" s="3"/>
       <c r="L175" s="3"/>
@@ -9020,7 +9028,7 @@
       <c r="Z176" s="3"/>
     </row>
     <row r="177" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="115"/>
+      <c r="A177" s="111"/>
       <c r="B177" s="28" t="s">
         <v>284</v>
       </c>
@@ -9064,7 +9072,7 @@
       <c r="Z177" s="3"/>
     </row>
     <row r="178" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="98"/>
+      <c r="A178" s="86"/>
       <c r="B178" s="30" t="s">
         <v>287</v>
       </c>
@@ -9108,7 +9116,7 @@
       <c r="Z178" s="3"/>
     </row>
     <row r="179" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="98"/>
+      <c r="A179" s="86"/>
       <c r="B179" s="30" t="s">
         <v>295</v>
       </c>
@@ -9152,7 +9160,7 @@
       <c r="Z179" s="3"/>
     </row>
     <row r="180" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="98"/>
+      <c r="A180" s="86"/>
       <c r="B180" s="30" t="s">
         <v>303</v>
       </c>
@@ -9196,7 +9204,7 @@
       <c r="Z180" s="3"/>
     </row>
     <row r="181" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="98"/>
+      <c r="A181" s="86"/>
       <c r="B181" s="30" t="s">
         <v>310</v>
       </c>
@@ -9240,7 +9248,7 @@
       <c r="Z181" s="3"/>
     </row>
     <row r="182" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="98"/>
+      <c r="A182" s="86"/>
       <c r="B182" s="30" t="s">
         <v>318</v>
       </c>
@@ -9284,7 +9292,7 @@
       <c r="Z182" s="3"/>
     </row>
     <row r="183" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="98"/>
+      <c r="A183" s="86"/>
       <c r="B183" s="30" t="s">
         <v>326</v>
       </c>
@@ -9328,7 +9336,7 @@
       <c r="Z183" s="3"/>
     </row>
     <row r="184" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="98"/>
+      <c r="A184" s="86"/>
       <c r="B184" s="30" t="s">
         <v>334</v>
       </c>
@@ -9372,7 +9380,7 @@
       <c r="Z184" s="3"/>
     </row>
     <row r="185" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="98"/>
+      <c r="A185" s="86"/>
       <c r="B185" s="30" t="s">
         <v>342</v>
       </c>
@@ -9416,7 +9424,7 @@
       <c r="Z185" s="3"/>
     </row>
     <row r="186" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="98"/>
+      <c r="A186" s="86"/>
       <c r="B186" s="30" t="s">
         <v>350</v>
       </c>
@@ -9460,7 +9468,7 @@
       <c r="Z186" s="3"/>
     </row>
     <row r="187" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="98"/>
+      <c r="A187" s="86"/>
       <c r="B187" s="30" t="s">
         <v>358</v>
       </c>
@@ -9504,7 +9512,7 @@
       <c r="Z187" s="3"/>
     </row>
     <row r="188" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="98"/>
+      <c r="A188" s="86"/>
       <c r="B188" s="30" t="s">
         <v>366</v>
       </c>
@@ -9548,7 +9556,7 @@
       <c r="Z188" s="3"/>
     </row>
     <row r="189" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="98"/>
+      <c r="A189" s="86"/>
       <c r="B189" s="30" t="s">
         <v>374</v>
       </c>
@@ -9592,7 +9600,7 @@
       <c r="Z189" s="3"/>
     </row>
     <row r="190" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="98"/>
+      <c r="A190" s="86"/>
       <c r="B190" s="30" t="s">
         <v>382</v>
       </c>
@@ -9636,7 +9644,7 @@
       <c r="Z190" s="3"/>
     </row>
     <row r="191" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="98"/>
+      <c r="A191" s="86"/>
       <c r="B191" s="30" t="s">
         <v>390</v>
       </c>
@@ -9674,7 +9682,7 @@
       <c r="Z191" s="3"/>
     </row>
     <row r="192" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="98"/>
+      <c r="A192" s="86"/>
       <c r="B192" s="30" t="s">
         <v>395</v>
       </c>
@@ -9714,7 +9722,7 @@
       <c r="Z192" s="3"/>
     </row>
     <row r="193" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="98"/>
+      <c r="A193" s="86"/>
       <c r="B193" s="30" t="s">
         <v>400</v>
       </c>
@@ -9754,7 +9762,7 @@
       <c r="Z193" s="3"/>
     </row>
     <row r="194" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="98"/>
+      <c r="A194" s="86"/>
       <c r="B194" s="30" t="s">
         <v>405</v>
       </c>
@@ -9794,7 +9802,7 @@
       <c r="Z194" s="3"/>
     </row>
     <row r="195" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="99"/>
+      <c r="A195" s="88"/>
       <c r="B195" s="30" t="s">
         <v>410</v>
       </c>
@@ -9862,17 +9870,17 @@
       <c r="Z196" s="3"/>
     </row>
     <row r="197" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="112" t="s">
+      <c r="A197" s="109" t="s">
         <v>415</v>
       </c>
-      <c r="B197" s="92"/>
-      <c r="C197" s="92"/>
-      <c r="D197" s="92"/>
-      <c r="E197" s="92"/>
-      <c r="F197" s="92"/>
-      <c r="G197" s="92"/>
-      <c r="H197" s="92"/>
-      <c r="I197" s="93"/>
+      <c r="B197" s="79"/>
+      <c r="C197" s="79"/>
+      <c r="D197" s="79"/>
+      <c r="E197" s="79"/>
+      <c r="F197" s="79"/>
+      <c r="G197" s="79"/>
+      <c r="H197" s="79"/>
+      <c r="I197" s="80"/>
       <c r="J197" s="2"/>
       <c r="K197" s="3"/>
       <c r="L197" s="3"/>
@@ -32427,17 +32435,176 @@
     </row>
   </sheetData>
   <mergeCells count="205">
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="A56:A83"/>
-    <mergeCell ref="E56:E83"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="A111:A135"/>
+    <mergeCell ref="E111:E135"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="B135:D135"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B132:D132"/>
+    <mergeCell ref="A137:A161"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B158:D158"/>
+    <mergeCell ref="B159:D159"/>
+    <mergeCell ref="B160:D160"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="F137:H137"/>
+    <mergeCell ref="F124:G124"/>
+    <mergeCell ref="H124:I124"/>
+    <mergeCell ref="F125:G125"/>
+    <mergeCell ref="H125:I125"/>
+    <mergeCell ref="F126:G126"/>
+    <mergeCell ref="H126:I126"/>
+    <mergeCell ref="H127:I127"/>
+    <mergeCell ref="H128:I128"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A3:A26"/>
+    <mergeCell ref="E3:E26"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="A28:A54"/>
+    <mergeCell ref="E28:E54"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B167:I167"/>
+    <mergeCell ref="B168:I168"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A163:I163"/>
+    <mergeCell ref="A165:I165"/>
+    <mergeCell ref="B166:I166"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="B153:C153"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D175:I175"/>
+    <mergeCell ref="A197:I197"/>
+    <mergeCell ref="B169:I169"/>
+    <mergeCell ref="B170:I170"/>
+    <mergeCell ref="B171:I171"/>
+    <mergeCell ref="A172:I172"/>
+    <mergeCell ref="A173:A175"/>
+    <mergeCell ref="D173:I173"/>
+    <mergeCell ref="D174:I174"/>
+    <mergeCell ref="A177:A195"/>
+    <mergeCell ref="F122:G122"/>
+    <mergeCell ref="H122:I122"/>
+    <mergeCell ref="F123:G123"/>
+    <mergeCell ref="H123:I123"/>
+    <mergeCell ref="B133:D133"/>
+    <mergeCell ref="B134:D134"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="F129:G129"/>
+    <mergeCell ref="H129:I129"/>
+    <mergeCell ref="F130:G130"/>
+    <mergeCell ref="F131:G131"/>
+    <mergeCell ref="F132:H132"/>
+    <mergeCell ref="F127:G127"/>
+    <mergeCell ref="F128:G128"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="B109:D109"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="A85:A109"/>
+    <mergeCell ref="E85:E109"/>
+    <mergeCell ref="H98:I98"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F98:G98"/>
+    <mergeCell ref="F99:G99"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="F103:G103"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="F104:G104"/>
+    <mergeCell ref="F106:G106"/>
     <mergeCell ref="C100:D100"/>
     <mergeCell ref="F100:G100"/>
     <mergeCell ref="H100:I100"/>
@@ -32462,176 +32629,17 @@
     <mergeCell ref="F78:G78"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="F79:G79"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="F103:G103"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="F104:G104"/>
-    <mergeCell ref="F106:G106"/>
-    <mergeCell ref="B107:D107"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="B109:D109"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="A85:A109"/>
-    <mergeCell ref="E85:E109"/>
-    <mergeCell ref="H98:I98"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F98:G98"/>
-    <mergeCell ref="F99:G99"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="F122:G122"/>
-    <mergeCell ref="H122:I122"/>
-    <mergeCell ref="F123:G123"/>
-    <mergeCell ref="H123:I123"/>
-    <mergeCell ref="B133:D133"/>
-    <mergeCell ref="B134:D134"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="F129:G129"/>
-    <mergeCell ref="H129:I129"/>
-    <mergeCell ref="F130:G130"/>
-    <mergeCell ref="F131:G131"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F127:G127"/>
-    <mergeCell ref="F128:G128"/>
-    <mergeCell ref="D175:I175"/>
-    <mergeCell ref="A197:I197"/>
-    <mergeCell ref="B169:I169"/>
-    <mergeCell ref="B170:I170"/>
-    <mergeCell ref="B171:I171"/>
-    <mergeCell ref="A172:I172"/>
-    <mergeCell ref="A173:A175"/>
-    <mergeCell ref="D173:I173"/>
-    <mergeCell ref="D174:I174"/>
-    <mergeCell ref="A177:A195"/>
-    <mergeCell ref="A163:I163"/>
-    <mergeCell ref="A165:I165"/>
-    <mergeCell ref="B166:I166"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="B153:C153"/>
-    <mergeCell ref="D153:E153"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="B167:I167"/>
-    <mergeCell ref="B168:I168"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="A3:A26"/>
-    <mergeCell ref="E3:E26"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="A28:A54"/>
-    <mergeCell ref="E28:E54"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="F137:H137"/>
-    <mergeCell ref="F124:G124"/>
-    <mergeCell ref="H124:I124"/>
-    <mergeCell ref="F125:G125"/>
-    <mergeCell ref="H125:I125"/>
-    <mergeCell ref="F126:G126"/>
-    <mergeCell ref="H126:I126"/>
-    <mergeCell ref="H127:I127"/>
-    <mergeCell ref="H128:I128"/>
-    <mergeCell ref="A111:A135"/>
-    <mergeCell ref="E111:E135"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="B135:D135"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B132:D132"/>
-    <mergeCell ref="A137:A161"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B158:D158"/>
-    <mergeCell ref="B159:D159"/>
-    <mergeCell ref="B160:D160"/>
-    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="A56:A83"/>
+    <mergeCell ref="E56:E83"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="F81:H81"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>